<commit_message>
post page ,my page, 옷장 분류 미완성
</commit_message>
<xml_diff>
--- a/산출물/api 명세서.xlsx
+++ b/산출물/api 명세서.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sw_engineering\SE2022-Team5\산출물\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1F9AC4-13C1-4F55-9C73-F6F2E008F07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A546E9-CAD0-4EAD-9AAE-DD1FE9D270D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API sheet - web client" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,15 @@
     <sheet name="3.2 - 게시물 생성" sheetId="9" r:id="rId7"/>
     <sheet name="3.3 - 게시물 수정" sheetId="10" r:id="rId8"/>
     <sheet name="3.4 - 게시물 삭제" sheetId="11" r:id="rId9"/>
+    <sheet name="4.1의상 조회" sheetId="12" r:id="rId10"/>
+    <sheet name="4.2 의상 생성" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="216">
   <si>
     <t>api 명세서에 x-access-token 부분은 10주차 이후에 적용되는 부분이니 넘어가주세요!</t>
   </si>
@@ -1010,6 +1012,214 @@
     <t>/clothes/clothesIdx/status</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>의상</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>조회</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> api</t>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>의상</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>생성</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> api</t>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>season</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bigCategory</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>smallCategory</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>color</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>img</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{
+    "isSuccess": true,
+    "code": 1000,
+    "message": "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>성공</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",
+    "result": {
+        "addedPost": 9
+    }
+}</t>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>ㄴ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>clothesIdx</t>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>추가된</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>옷</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> idx</t>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1018,7 +1228,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="m\ d"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="33">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1209,6 +1419,29 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -1325,7 +1558,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1479,6 +1712,15 @@
     <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1853,16 +2095,16 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="13">
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="79"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="84"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="84"/>
     </row>
     <row r="8" spans="2:12" ht="15.75" customHeight="1">
       <c r="B8" s="18">
@@ -1931,16 +2173,16 @@
       <c r="I10" s="19"/>
     </row>
     <row r="11" spans="2:12" ht="15.75" customHeight="1">
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="79"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="79"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="84"/>
+      <c r="E11" s="84"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="84"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="84"/>
     </row>
     <row r="12" spans="2:12" ht="12.5">
       <c r="B12" s="18">
@@ -1965,16 +2207,16 @@
       <c r="I12" s="19"/>
     </row>
     <row r="13" spans="2:12" ht="15.75" customHeight="1">
-      <c r="B13" s="79" t="s">
+      <c r="B13" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="79"/>
-      <c r="D13" s="79"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="79"/>
-      <c r="G13" s="79"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="79"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="84"/>
+      <c r="F13" s="84"/>
+      <c r="G13" s="84"/>
+      <c r="H13" s="84"/>
+      <c r="I13" s="84"/>
     </row>
     <row r="14" spans="2:12" ht="15.75" customHeight="1">
       <c r="B14" s="18">
@@ -2083,16 +2325,16 @@
       <c r="Z17" s="27"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1">
-      <c r="B18" s="78" t="s">
+      <c r="B18" s="83" t="s">
         <v>195</v>
       </c>
-      <c r="C18" s="78"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="78"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="78"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="78"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="83"/>
+      <c r="G18" s="83"/>
+      <c r="H18" s="83"/>
+      <c r="I18" s="83"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1">
       <c r="A19" s="24"/>
@@ -2277,14 +2519,14 @@
       <c r="I23" s="19"/>
     </row>
     <row r="24" spans="1:26" ht="13">
-      <c r="B24" s="77"/>
-      <c r="C24" s="77"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="77"/>
-      <c r="G24" s="77"/>
-      <c r="H24" s="77"/>
-      <c r="I24" s="77"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="82"/>
+      <c r="G24" s="82"/>
+      <c r="H24" s="82"/>
+      <c r="I24" s="82"/>
     </row>
     <row r="25" spans="1:26" ht="12.5">
       <c r="A25" s="12"/>
@@ -7249,6 +7491,1998 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E854DB-8757-4DC5-AF99-902D7EFA66F4}">
+  <dimension ref="A1:H94"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:H37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5"/>
+  <cols>
+    <col min="2" max="2" width="19.36328125" customWidth="1"/>
+    <col min="3" max="3" width="16.08984375" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="15.90625" customWidth="1"/>
+    <col min="8" max="8" width="21.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="16">
+      <c r="A1" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="78" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="70" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="77"/>
+      <c r="B3" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="77" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="77"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="77"/>
+      <c r="B5" s="77" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="77"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="77"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="77" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="77"/>
+      <c r="B8" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="77"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="77"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="77"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="77"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="77"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="77"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="77"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="77"/>
+      <c r="B13" s="77" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="77"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="63"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="77"/>
+      <c r="B15" s="77"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="77"/>
+      <c r="H15" s="77"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="77"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="77"/>
+      <c r="H16" s="77"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="77"/>
+      <c r="B17" s="77" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="77"/>
+      <c r="B18" s="77"/>
+      <c r="C18" s="77"/>
+      <c r="D18" s="77"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="77"/>
+      <c r="G18" s="77"/>
+      <c r="H18" s="77"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="77"/>
+      <c r="B19" s="77"/>
+      <c r="C19" s="77"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="77"/>
+      <c r="H19" s="77"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="77"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="77"/>
+      <c r="H20" s="77"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="77"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="77"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="77"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="77"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="77"/>
+      <c r="H22" s="77"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="77"/>
+      <c r="B23" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="77"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="77"/>
+      <c r="H23" s="77"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="77"/>
+      <c r="B24" s="77"/>
+      <c r="C24" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="77"/>
+      <c r="B25" s="77"/>
+      <c r="C25" s="77"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="77"/>
+      <c r="H25" s="77"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="77"/>
+      <c r="B26" s="77"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="77"/>
+      <c r="H26" s="77"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="77"/>
+      <c r="B27" s="77"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="77"/>
+      <c r="H27" s="77"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="77"/>
+      <c r="B28" s="77"/>
+      <c r="C28" s="77"/>
+      <c r="D28" s="77"/>
+      <c r="E28" s="77"/>
+      <c r="F28" s="77"/>
+      <c r="G28" s="77"/>
+      <c r="H28" s="77"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="77"/>
+      <c r="B29" s="77"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="77"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="77"/>
+      <c r="H29" s="77"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="77"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="77"/>
+      <c r="H30" s="77"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="77"/>
+      <c r="B31" s="77"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="77"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="77"/>
+      <c r="B32" s="77"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="77"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="77"/>
+      <c r="H32" s="77"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="77"/>
+      <c r="B33" s="77"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="77"/>
+      <c r="H33" s="77"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="77"/>
+      <c r="B34" s="77"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="77"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="77"/>
+      <c r="B35" s="77"/>
+      <c r="C35" s="77"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="77"/>
+      <c r="G35" s="77"/>
+      <c r="H35" s="77"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="77"/>
+      <c r="B36" s="77"/>
+      <c r="C36" s="77"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="77"/>
+      <c r="G36" s="77"/>
+      <c r="H36" s="77"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="77"/>
+      <c r="B37" s="77"/>
+      <c r="C37" s="77"/>
+      <c r="D37" s="77"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="77"/>
+      <c r="G37" s="77"/>
+      <c r="H37" s="77"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="77"/>
+      <c r="B38" s="77"/>
+      <c r="C38" s="77"/>
+      <c r="D38" s="77"/>
+      <c r="E38" s="77"/>
+      <c r="F38" s="77"/>
+      <c r="G38" s="77"/>
+      <c r="H38" s="77"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="77"/>
+      <c r="B39" s="77"/>
+      <c r="C39" s="77"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="77"/>
+      <c r="G39" s="77"/>
+      <c r="H39" s="77"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="77"/>
+      <c r="B40" s="77"/>
+      <c r="C40" s="77" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="77" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40" s="77" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" s="77"/>
+      <c r="H40" s="77" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="77"/>
+      <c r="B41" s="77"/>
+      <c r="C41" s="77" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="E41" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" s="47">
+        <v>1000</v>
+      </c>
+      <c r="G41" s="77"/>
+      <c r="H41" s="77" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="77"/>
+      <c r="B42" s="77"/>
+      <c r="C42" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="77" t="s">
+        <v>71</v>
+      </c>
+      <c r="G42" s="77"/>
+      <c r="H42" s="77" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="77"/>
+      <c r="B43" s="77"/>
+      <c r="C43" s="77"/>
+      <c r="D43" s="77"/>
+      <c r="E43" s="77"/>
+      <c r="F43" s="77"/>
+      <c r="G43" s="77"/>
+      <c r="H43" s="77"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="77"/>
+      <c r="B44" s="77"/>
+      <c r="C44" s="77"/>
+      <c r="D44" s="77"/>
+      <c r="E44" s="77"/>
+      <c r="F44" s="77"/>
+      <c r="G44" s="77"/>
+      <c r="H44" s="77"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="77"/>
+      <c r="B45" s="77"/>
+      <c r="C45" s="77"/>
+      <c r="D45" s="77"/>
+      <c r="E45" s="77"/>
+      <c r="F45" s="77"/>
+      <c r="G45" s="77"/>
+      <c r="H45" s="77"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="77"/>
+      <c r="B46" s="77"/>
+      <c r="C46" s="77"/>
+      <c r="D46" s="77"/>
+      <c r="E46" s="77"/>
+      <c r="F46" s="77"/>
+      <c r="G46" s="77"/>
+      <c r="H46" s="77"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="77"/>
+      <c r="B47" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" s="77"/>
+      <c r="D47" s="77"/>
+      <c r="E47" s="77"/>
+      <c r="F47" s="77"/>
+      <c r="G47" s="77"/>
+      <c r="H47" s="77"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="77"/>
+      <c r="B48" s="77"/>
+      <c r="C48" s="85" t="s">
+        <v>152</v>
+      </c>
+      <c r="D48" s="86"/>
+      <c r="E48" s="86"/>
+      <c r="F48" s="86"/>
+      <c r="G48" s="77"/>
+      <c r="H48" s="77"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="77"/>
+      <c r="B49" s="77"/>
+      <c r="C49" s="86"/>
+      <c r="D49" s="86"/>
+      <c r="E49" s="86"/>
+      <c r="F49" s="86"/>
+      <c r="G49" s="77"/>
+      <c r="H49" s="77"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="77"/>
+      <c r="B50" s="77"/>
+      <c r="C50" s="86"/>
+      <c r="D50" s="86"/>
+      <c r="E50" s="86"/>
+      <c r="F50" s="86"/>
+      <c r="G50" s="77"/>
+      <c r="H50" s="77"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="77"/>
+      <c r="B51" s="77"/>
+      <c r="C51" s="86"/>
+      <c r="D51" s="86"/>
+      <c r="E51" s="86"/>
+      <c r="F51" s="86"/>
+      <c r="G51" s="77"/>
+      <c r="H51" s="77"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="77"/>
+      <c r="B52" s="77"/>
+      <c r="C52" s="86"/>
+      <c r="D52" s="86"/>
+      <c r="E52" s="86"/>
+      <c r="F52" s="86"/>
+      <c r="G52" s="77"/>
+      <c r="H52" s="77"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="77"/>
+      <c r="B53" s="77"/>
+      <c r="C53" s="86"/>
+      <c r="D53" s="86"/>
+      <c r="E53" s="86"/>
+      <c r="F53" s="86"/>
+      <c r="G53" s="77"/>
+      <c r="H53" s="77"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="77"/>
+      <c r="B54" s="77"/>
+      <c r="C54" s="86"/>
+      <c r="D54" s="86"/>
+      <c r="E54" s="86"/>
+      <c r="F54" s="86"/>
+      <c r="G54" s="77"/>
+      <c r="H54" s="77"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="77"/>
+      <c r="B55" s="77"/>
+      <c r="C55" s="86"/>
+      <c r="D55" s="86"/>
+      <c r="E55" s="86"/>
+      <c r="F55" s="86"/>
+      <c r="G55" s="77"/>
+      <c r="H55" s="77"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="77"/>
+      <c r="B56" s="77"/>
+      <c r="C56" s="86"/>
+      <c r="D56" s="86"/>
+      <c r="E56" s="86"/>
+      <c r="F56" s="86"/>
+      <c r="G56" s="77"/>
+      <c r="H56" s="77"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="77"/>
+      <c r="B57" s="77"/>
+      <c r="C57" s="86"/>
+      <c r="D57" s="86"/>
+      <c r="E57" s="86"/>
+      <c r="F57" s="86"/>
+      <c r="G57" s="77"/>
+      <c r="H57" s="77"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="77"/>
+      <c r="B58" s="77"/>
+      <c r="C58" s="86"/>
+      <c r="D58" s="86"/>
+      <c r="E58" s="86"/>
+      <c r="F58" s="86"/>
+      <c r="G58" s="77"/>
+      <c r="H58" s="77"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="77"/>
+      <c r="B59" s="77"/>
+      <c r="C59" s="86"/>
+      <c r="D59" s="86"/>
+      <c r="E59" s="86"/>
+      <c r="F59" s="86"/>
+      <c r="G59" s="77"/>
+      <c r="H59" s="77"/>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="77"/>
+      <c r="B60" s="77"/>
+      <c r="C60" s="86"/>
+      <c r="D60" s="86"/>
+      <c r="E60" s="86"/>
+      <c r="F60" s="86"/>
+      <c r="G60" s="77"/>
+      <c r="H60" s="77"/>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="77"/>
+      <c r="B61" s="77"/>
+      <c r="C61" s="86"/>
+      <c r="D61" s="86"/>
+      <c r="E61" s="86"/>
+      <c r="F61" s="86"/>
+      <c r="G61" s="77"/>
+      <c r="H61" s="77"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="77"/>
+      <c r="B62" s="77"/>
+      <c r="C62" s="86"/>
+      <c r="D62" s="86"/>
+      <c r="E62" s="86"/>
+      <c r="F62" s="86"/>
+      <c r="G62" s="77"/>
+      <c r="H62" s="77"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="77"/>
+      <c r="B63" s="77"/>
+      <c r="C63" s="86"/>
+      <c r="D63" s="86"/>
+      <c r="E63" s="86"/>
+      <c r="F63" s="86"/>
+      <c r="G63" s="77"/>
+      <c r="H63" s="77"/>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="77"/>
+      <c r="B64" s="77"/>
+      <c r="C64" s="86"/>
+      <c r="D64" s="86"/>
+      <c r="E64" s="86"/>
+      <c r="F64" s="86"/>
+      <c r="G64" s="77"/>
+      <c r="H64" s="77"/>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="77"/>
+      <c r="B65" s="77"/>
+      <c r="C65" s="86"/>
+      <c r="D65" s="86"/>
+      <c r="E65" s="86"/>
+      <c r="F65" s="86"/>
+      <c r="G65" s="77"/>
+      <c r="H65" s="77"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="77"/>
+      <c r="B66" s="77"/>
+      <c r="C66" s="86"/>
+      <c r="D66" s="86"/>
+      <c r="E66" s="86"/>
+      <c r="F66" s="86"/>
+      <c r="G66" s="77"/>
+      <c r="H66" s="77"/>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="77"/>
+      <c r="B67" s="77"/>
+      <c r="C67" s="86"/>
+      <c r="D67" s="86"/>
+      <c r="E67" s="86"/>
+      <c r="F67" s="86"/>
+      <c r="G67" s="77"/>
+      <c r="H67" s="77"/>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="77"/>
+      <c r="B68" s="77"/>
+      <c r="C68" s="86"/>
+      <c r="D68" s="86"/>
+      <c r="E68" s="86"/>
+      <c r="F68" s="86"/>
+      <c r="G68" s="77"/>
+      <c r="H68" s="77"/>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="77"/>
+      <c r="B69" s="77"/>
+      <c r="C69" s="86"/>
+      <c r="D69" s="86"/>
+      <c r="E69" s="86"/>
+      <c r="F69" s="86"/>
+      <c r="G69" s="77"/>
+      <c r="H69" s="77"/>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="77"/>
+      <c r="B70" s="77"/>
+      <c r="C70" s="86"/>
+      <c r="D70" s="86"/>
+      <c r="E70" s="86"/>
+      <c r="F70" s="86"/>
+      <c r="G70" s="77"/>
+      <c r="H70" s="77"/>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="77"/>
+      <c r="B71" s="77"/>
+      <c r="C71" s="86"/>
+      <c r="D71" s="86"/>
+      <c r="E71" s="86"/>
+      <c r="F71" s="86"/>
+      <c r="G71" s="77"/>
+      <c r="H71" s="77"/>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="77"/>
+      <c r="B72" s="77"/>
+      <c r="C72" s="86"/>
+      <c r="D72" s="86"/>
+      <c r="E72" s="86"/>
+      <c r="F72" s="86"/>
+      <c r="G72" s="77"/>
+      <c r="H72" s="77"/>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="77"/>
+      <c r="B73" s="77"/>
+      <c r="C73" s="86"/>
+      <c r="D73" s="86"/>
+      <c r="E73" s="86"/>
+      <c r="F73" s="86"/>
+      <c r="G73" s="77"/>
+      <c r="H73" s="77"/>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="77"/>
+      <c r="B74" s="77"/>
+      <c r="C74" s="86"/>
+      <c r="D74" s="86"/>
+      <c r="E74" s="86"/>
+      <c r="F74" s="86"/>
+      <c r="G74" s="77"/>
+      <c r="H74" s="77"/>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="77"/>
+      <c r="B75" s="77"/>
+      <c r="C75" s="86"/>
+      <c r="D75" s="86"/>
+      <c r="E75" s="86"/>
+      <c r="F75" s="86"/>
+      <c r="G75" s="77"/>
+      <c r="H75" s="77"/>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="77"/>
+      <c r="B76" s="77"/>
+      <c r="C76" s="86"/>
+      <c r="D76" s="86"/>
+      <c r="E76" s="86"/>
+      <c r="F76" s="86"/>
+      <c r="G76" s="77"/>
+      <c r="H76" s="77"/>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="77"/>
+      <c r="B77" s="77"/>
+      <c r="C77" s="86"/>
+      <c r="D77" s="86"/>
+      <c r="E77" s="86"/>
+      <c r="F77" s="86"/>
+      <c r="G77" s="77"/>
+      <c r="H77" s="77"/>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="77"/>
+      <c r="B78" s="77"/>
+      <c r="C78" s="86"/>
+      <c r="D78" s="86"/>
+      <c r="E78" s="86"/>
+      <c r="F78" s="86"/>
+      <c r="G78" s="77"/>
+      <c r="H78" s="77"/>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" s="77"/>
+      <c r="B79" s="77"/>
+      <c r="C79" s="86"/>
+      <c r="D79" s="86"/>
+      <c r="E79" s="86"/>
+      <c r="F79" s="86"/>
+      <c r="G79" s="77"/>
+      <c r="H79" s="77"/>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="77"/>
+      <c r="B80" s="77"/>
+      <c r="C80" s="86"/>
+      <c r="D80" s="86"/>
+      <c r="E80" s="86"/>
+      <c r="F80" s="86"/>
+      <c r="G80" s="77"/>
+      <c r="H80" s="77"/>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" s="77"/>
+      <c r="B81" s="77"/>
+      <c r="C81" s="86"/>
+      <c r="D81" s="86"/>
+      <c r="E81" s="86"/>
+      <c r="F81" s="86"/>
+      <c r="G81" s="77"/>
+      <c r="H81" s="77"/>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" s="77"/>
+      <c r="B82" s="77"/>
+      <c r="C82" s="86"/>
+      <c r="D82" s="86"/>
+      <c r="E82" s="86"/>
+      <c r="F82" s="86"/>
+      <c r="G82" s="77"/>
+      <c r="H82" s="77"/>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" s="77"/>
+      <c r="B83" s="77"/>
+      <c r="C83" s="86"/>
+      <c r="D83" s="86"/>
+      <c r="E83" s="86"/>
+      <c r="F83" s="86"/>
+      <c r="G83" s="77"/>
+      <c r="H83" s="77"/>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" s="77"/>
+      <c r="B84" s="77"/>
+      <c r="C84" s="86"/>
+      <c r="D84" s="86"/>
+      <c r="E84" s="86"/>
+      <c r="F84" s="86"/>
+      <c r="G84" s="77"/>
+      <c r="H84" s="77"/>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" s="77"/>
+      <c r="B85" s="77"/>
+      <c r="C85" s="86"/>
+      <c r="D85" s="86"/>
+      <c r="E85" s="86"/>
+      <c r="F85" s="86"/>
+      <c r="G85" s="77"/>
+      <c r="H85" s="77"/>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="77"/>
+      <c r="B86" s="77"/>
+      <c r="C86" s="86"/>
+      <c r="D86" s="86"/>
+      <c r="E86" s="86"/>
+      <c r="F86" s="86"/>
+      <c r="G86" s="77"/>
+      <c r="H86" s="77"/>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" s="77"/>
+      <c r="B87" s="77"/>
+      <c r="C87" s="77"/>
+      <c r="D87" s="77"/>
+      <c r="E87" s="77"/>
+      <c r="F87" s="77"/>
+      <c r="G87" s="77"/>
+      <c r="H87" s="77"/>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" s="77"/>
+      <c r="B88" s="77" t="s">
+        <v>75</v>
+      </c>
+      <c r="C88" s="77"/>
+      <c r="D88" s="77"/>
+      <c r="E88" s="77"/>
+      <c r="F88" s="77"/>
+      <c r="G88" s="77"/>
+      <c r="H88" s="77"/>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" s="77"/>
+      <c r="B89" s="77"/>
+      <c r="C89" s="77" t="s">
+        <v>67</v>
+      </c>
+      <c r="D89" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="E89" s="77"/>
+      <c r="F89" s="77"/>
+      <c r="G89" s="77"/>
+      <c r="H89" s="77"/>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" s="77"/>
+      <c r="B90" s="77"/>
+      <c r="C90" s="44">
+        <v>200</v>
+      </c>
+      <c r="D90" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="E90" s="77"/>
+      <c r="F90" s="77"/>
+      <c r="G90" s="77"/>
+      <c r="H90" s="77"/>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" s="77"/>
+      <c r="B91" s="77"/>
+      <c r="C91" s="47">
+        <v>1000</v>
+      </c>
+      <c r="D91" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="E91" s="77"/>
+      <c r="F91" s="77"/>
+      <c r="G91" s="77"/>
+      <c r="H91" s="77"/>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" s="77"/>
+      <c r="B92" s="77"/>
+      <c r="C92" s="47">
+        <v>2000</v>
+      </c>
+      <c r="D92" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="E92" s="77"/>
+      <c r="F92" s="77"/>
+      <c r="G92" s="77"/>
+      <c r="H92" s="77"/>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="A93" s="77"/>
+      <c r="B93" s="77"/>
+      <c r="C93" s="47">
+        <v>2002</v>
+      </c>
+      <c r="D93" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="E93" s="77"/>
+      <c r="F93" s="77"/>
+      <c r="G93" s="77"/>
+      <c r="H93" s="77"/>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" s="77"/>
+      <c r="B94" s="77"/>
+      <c r="C94" s="47">
+        <v>4000</v>
+      </c>
+      <c r="D94" s="77" t="s">
+        <v>89</v>
+      </c>
+      <c r="E94" s="77"/>
+      <c r="F94" s="77"/>
+      <c r="G94" s="77"/>
+      <c r="H94" s="77"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C48:F86"/>
+  </mergeCells>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C1" location="API sheet - web client!A1" display="API 인덱스" xr:uid="{B2D102EA-70EC-4546-8735-C0483B642683}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D501B46-09FD-4FC4-A14B-B443CDCE76FA}">
+  <dimension ref="A1:I58"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I27" sqref="I26:I27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="10.453125" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" customWidth="1"/>
+    <col min="6" max="6" width="19.6328125" customWidth="1"/>
+    <col min="7" max="7" width="12.90625" customWidth="1"/>
+    <col min="8" max="8" width="21.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16">
+      <c r="A1" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="79" t="s">
+        <v>206</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="77" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="77"/>
+      <c r="B3" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="77" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="77"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="77"/>
+      <c r="B5" s="77" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="77"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="77"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="77"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="77" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="I7" s="77"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="77"/>
+      <c r="B8" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="77"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="77"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="77"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="D10" s="70" t="s">
+        <v>182</v>
+      </c>
+      <c r="E10" s="70" t="s">
+        <v>180</v>
+      </c>
+      <c r="F10" s="77"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="77" t="s">
+        <v>154</v>
+      </c>
+      <c r="I10" s="77"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="77"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="70" t="s">
+        <v>207</v>
+      </c>
+      <c r="D11" s="70" t="s">
+        <v>212</v>
+      </c>
+      <c r="E11" s="70" t="s">
+        <v>180</v>
+      </c>
+      <c r="F11" s="77"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="77" t="s">
+        <v>157</v>
+      </c>
+      <c r="I11" s="77"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="77"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="70" t="s">
+        <v>208</v>
+      </c>
+      <c r="D12" s="70" t="s">
+        <v>212</v>
+      </c>
+      <c r="E12" s="70" t="s">
+        <v>180</v>
+      </c>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="77"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="77"/>
+      <c r="B13" s="77"/>
+      <c r="C13" s="70" t="s">
+        <v>209</v>
+      </c>
+      <c r="D13" s="70" t="s">
+        <v>212</v>
+      </c>
+      <c r="E13" s="70" t="s">
+        <v>180</v>
+      </c>
+      <c r="F13" s="77"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="77"/>
+      <c r="I13" s="77"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="77"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="70" t="s">
+        <v>210</v>
+      </c>
+      <c r="D14" s="70" t="s">
+        <v>182</v>
+      </c>
+      <c r="E14" s="70" t="s">
+        <v>180</v>
+      </c>
+      <c r="F14" s="77"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="77"/>
+      <c r="I14" s="77"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="77"/>
+      <c r="B15" s="77"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="77"/>
+      <c r="H15" s="77"/>
+      <c r="I15" s="77"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="77"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="77"/>
+      <c r="H16" s="77"/>
+      <c r="I16" s="77"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="77"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="77"/>
+      <c r="H17" s="77"/>
+      <c r="I17" s="77"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="77"/>
+      <c r="B18" s="77" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="77"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="77"/>
+      <c r="B19" s="77"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="57"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="77"/>
+      <c r="B20" s="77"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="77"/>
+      <c r="H20" s="77"/>
+      <c r="I20" s="77"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="77"/>
+      <c r="B21" s="77"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="77"/>
+      <c r="I21" s="77"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="77"/>
+      <c r="B22" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="77"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="77"/>
+      <c r="H22" s="77"/>
+      <c r="I22" s="77"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="77"/>
+      <c r="B23" s="77"/>
+      <c r="C23" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="77"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="77"/>
+      <c r="B24" s="77"/>
+      <c r="C24" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="77"/>
+      <c r="G24" s="77"/>
+      <c r="H24" s="77"/>
+      <c r="I24" s="77"/>
+    </row>
+    <row r="25" spans="1:9" ht="16">
+      <c r="A25" s="77"/>
+      <c r="B25" s="77"/>
+      <c r="C25" s="80" t="s">
+        <v>214</v>
+      </c>
+      <c r="D25" s="77" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" s="77"/>
+      <c r="G25" s="77"/>
+      <c r="H25" s="81" t="s">
+        <v>215</v>
+      </c>
+      <c r="I25" s="77"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="77"/>
+      <c r="B26" s="77"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="77"/>
+      <c r="H26" s="77"/>
+      <c r="I26" s="77"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="77"/>
+      <c r="B27" s="77"/>
+      <c r="C27" s="77" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="77" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="77" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" s="77"/>
+      <c r="H27" s="77" t="s">
+        <v>66</v>
+      </c>
+      <c r="I27" s="77"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="77"/>
+      <c r="B28" s="77"/>
+      <c r="C28" s="77" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="47">
+        <v>1000</v>
+      </c>
+      <c r="G28" s="77"/>
+      <c r="H28" s="77" t="s">
+        <v>69</v>
+      </c>
+      <c r="I28" s="77"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="77"/>
+      <c r="B29" s="77"/>
+      <c r="C29" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" s="77" t="s">
+        <v>71</v>
+      </c>
+      <c r="G29" s="77"/>
+      <c r="H29" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="I29" s="77"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="77"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="77"/>
+      <c r="H30" s="77"/>
+      <c r="I30" s="77"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="77"/>
+      <c r="B31" s="77"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="77"/>
+      <c r="I31" s="77"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="77"/>
+      <c r="B32" s="77"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="77"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="77"/>
+      <c r="H32" s="77"/>
+      <c r="I32" s="77"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="77"/>
+      <c r="B33" s="77"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="77"/>
+      <c r="H33" s="77"/>
+      <c r="I33" s="77"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="77"/>
+      <c r="B34" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="77"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="77"/>
+      <c r="B35" s="77"/>
+      <c r="C35" s="85" t="s">
+        <v>160</v>
+      </c>
+      <c r="D35" s="86"/>
+      <c r="E35" s="86"/>
+      <c r="F35" s="86"/>
+      <c r="G35" s="77"/>
+      <c r="H35" s="77"/>
+      <c r="I35" s="77"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="77"/>
+      <c r="B36" s="77"/>
+      <c r="C36" s="86"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="86"/>
+      <c r="F36" s="86"/>
+      <c r="G36" s="77"/>
+      <c r="H36" s="77"/>
+      <c r="I36" s="77"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="77"/>
+      <c r="B37" s="77"/>
+      <c r="C37" s="86"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="86"/>
+      <c r="F37" s="86"/>
+      <c r="G37" s="77"/>
+      <c r="H37" s="77"/>
+      <c r="I37" s="77"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="77"/>
+      <c r="B38" s="77"/>
+      <c r="C38" s="86"/>
+      <c r="D38" s="86"/>
+      <c r="E38" s="86"/>
+      <c r="F38" s="86"/>
+      <c r="G38" s="77"/>
+      <c r="H38" s="77"/>
+      <c r="I38" s="77"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="77"/>
+      <c r="B39" s="77"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="86"/>
+      <c r="F39" s="86"/>
+      <c r="G39" s="77"/>
+      <c r="H39" s="77"/>
+      <c r="I39" s="77"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="77"/>
+      <c r="B40" s="77"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="86"/>
+      <c r="E40" s="86"/>
+      <c r="F40" s="86"/>
+      <c r="G40" s="77"/>
+      <c r="H40" s="77"/>
+      <c r="I40" s="77"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="77"/>
+      <c r="B41" s="77"/>
+      <c r="C41" s="86"/>
+      <c r="D41" s="86"/>
+      <c r="E41" s="86"/>
+      <c r="F41" s="86"/>
+      <c r="G41" s="77"/>
+      <c r="H41" s="77"/>
+      <c r="I41" s="77"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="77"/>
+      <c r="B42" s="77"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="86"/>
+      <c r="E42" s="86"/>
+      <c r="F42" s="86"/>
+      <c r="G42" s="77"/>
+      <c r="H42" s="77"/>
+      <c r="I42" s="77"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="77"/>
+      <c r="B43" s="77"/>
+      <c r="C43" s="86"/>
+      <c r="D43" s="86"/>
+      <c r="E43" s="86"/>
+      <c r="F43" s="86"/>
+      <c r="G43" s="77"/>
+      <c r="H43" s="77"/>
+      <c r="I43" s="77"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="77"/>
+      <c r="B44" s="77"/>
+      <c r="C44" s="86"/>
+      <c r="D44" s="86"/>
+      <c r="E44" s="86"/>
+      <c r="F44" s="86"/>
+      <c r="G44" s="77"/>
+      <c r="H44" s="77"/>
+      <c r="I44" s="77"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="77"/>
+      <c r="B45" s="77"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="86"/>
+      <c r="F45" s="86"/>
+      <c r="G45" s="77"/>
+      <c r="H45" s="77"/>
+      <c r="I45" s="77"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="77"/>
+      <c r="B46" s="77"/>
+      <c r="C46" s="86"/>
+      <c r="D46" s="86"/>
+      <c r="E46" s="86"/>
+      <c r="F46" s="86"/>
+      <c r="G46" s="77"/>
+      <c r="H46" s="77"/>
+      <c r="I46" s="77"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="77"/>
+      <c r="B47" s="77"/>
+      <c r="C47" s="86"/>
+      <c r="D47" s="86"/>
+      <c r="E47" s="86"/>
+      <c r="F47" s="86"/>
+      <c r="G47" s="77"/>
+      <c r="H47" s="77"/>
+      <c r="I47" s="77"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="77"/>
+      <c r="B48" s="77" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" s="77"/>
+      <c r="D48" s="77"/>
+      <c r="E48" s="77"/>
+      <c r="F48" s="77"/>
+      <c r="G48" s="77"/>
+      <c r="H48" s="77"/>
+      <c r="I48" s="77"/>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="77"/>
+      <c r="B49" s="77"/>
+      <c r="C49" s="77" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="E49" s="77"/>
+      <c r="F49" s="77"/>
+      <c r="G49" s="77"/>
+      <c r="H49" s="77"/>
+      <c r="I49" s="77"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="77"/>
+      <c r="B50" s="77"/>
+      <c r="C50" s="44">
+        <v>200</v>
+      </c>
+      <c r="D50" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="E50" s="77"/>
+      <c r="F50" s="77"/>
+      <c r="G50" s="77"/>
+      <c r="H50" s="77"/>
+      <c r="I50" s="77"/>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="77"/>
+      <c r="B51" s="77"/>
+      <c r="C51" s="47">
+        <v>1000</v>
+      </c>
+      <c r="D51" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="E51" s="77"/>
+      <c r="F51" s="77"/>
+      <c r="G51" s="77"/>
+      <c r="H51" s="77"/>
+      <c r="I51" s="77"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="77"/>
+      <c r="B52" s="77"/>
+      <c r="C52" s="47">
+        <v>2000</v>
+      </c>
+      <c r="D52" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="E52" s="77"/>
+      <c r="F52" s="77"/>
+      <c r="G52" s="77"/>
+      <c r="H52" s="77"/>
+      <c r="I52" s="77"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="77"/>
+      <c r="B53" s="77"/>
+      <c r="C53" s="47">
+        <v>2002</v>
+      </c>
+      <c r="D53" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="E53" s="77"/>
+      <c r="F53" s="77"/>
+      <c r="G53" s="77"/>
+      <c r="H53" s="77"/>
+      <c r="I53" s="77"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="77"/>
+      <c r="B54" s="77"/>
+      <c r="C54" s="47">
+        <v>2010</v>
+      </c>
+      <c r="D54" s="77" t="s">
+        <v>104</v>
+      </c>
+      <c r="E54" s="77"/>
+      <c r="F54" s="77"/>
+      <c r="G54" s="77"/>
+      <c r="H54" s="77"/>
+      <c r="I54" s="77"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="77"/>
+      <c r="B55" s="77"/>
+      <c r="C55" s="47">
+        <v>2040</v>
+      </c>
+      <c r="D55" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="E55" s="77"/>
+      <c r="F55" s="77"/>
+      <c r="G55" s="77"/>
+      <c r="H55" s="77"/>
+      <c r="I55" s="77"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="77"/>
+      <c r="B56" s="77"/>
+      <c r="C56" s="47">
+        <v>2041</v>
+      </c>
+      <c r="D56" s="77" t="s">
+        <v>162</v>
+      </c>
+      <c r="E56" s="77"/>
+      <c r="F56" s="77"/>
+      <c r="G56" s="77"/>
+      <c r="H56" s="77"/>
+      <c r="I56" s="77"/>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="77"/>
+      <c r="B57" s="77"/>
+      <c r="C57" s="47">
+        <v>2042</v>
+      </c>
+      <c r="D57" s="77" t="s">
+        <v>163</v>
+      </c>
+      <c r="E57" s="77"/>
+      <c r="F57" s="77"/>
+      <c r="G57" s="77"/>
+      <c r="H57" s="77"/>
+      <c r="I57" s="77"/>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="77"/>
+      <c r="B58" s="77"/>
+      <c r="C58" s="47">
+        <v>4000</v>
+      </c>
+      <c r="D58" s="77" t="s">
+        <v>89</v>
+      </c>
+      <c r="E58" s="77"/>
+      <c r="F58" s="77"/>
+      <c r="G58" s="77"/>
+      <c r="H58" s="77"/>
+      <c r="I58" s="77"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C35:F47"/>
+  </mergeCells>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C1" location="API sheet - web client!A1" display="API 인덱스" xr:uid="{B3F6B831-5E48-4197-AE0A-D55873E758B9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
@@ -7256,7 +9490,7 @@
   </sheetPr>
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -7928,12 +10162,12 @@
     <row r="39" spans="1:11" ht="13">
       <c r="A39" s="34"/>
       <c r="B39" s="34"/>
-      <c r="C39" s="80" t="s">
+      <c r="C39" s="85" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="86"/>
+      <c r="F39" s="86"/>
       <c r="G39" s="34"/>
       <c r="H39" s="34"/>
       <c r="I39" s="34"/>
@@ -7943,10 +10177,10 @@
     <row r="40" spans="1:11" ht="13">
       <c r="A40" s="34"/>
       <c r="B40" s="34"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="81"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="86"/>
+      <c r="E40" s="86"/>
+      <c r="F40" s="86"/>
       <c r="G40" s="34"/>
       <c r="H40" s="34"/>
       <c r="I40" s="34"/>
@@ -7956,10 +10190,10 @@
     <row r="41" spans="1:11" ht="13">
       <c r="A41" s="34"/>
       <c r="B41" s="34"/>
-      <c r="C41" s="81"/>
-      <c r="D41" s="81"/>
-      <c r="E41" s="81"/>
-      <c r="F41" s="81"/>
+      <c r="C41" s="86"/>
+      <c r="D41" s="86"/>
+      <c r="E41" s="86"/>
+      <c r="F41" s="86"/>
       <c r="G41" s="34"/>
       <c r="H41" s="34"/>
       <c r="I41" s="34"/>
@@ -7969,10 +10203,10 @@
     <row r="42" spans="1:11" ht="15.75" customHeight="1">
       <c r="A42" s="34"/>
       <c r="B42" s="34"/>
-      <c r="C42" s="81"/>
-      <c r="D42" s="81"/>
-      <c r="E42" s="81"/>
-      <c r="F42" s="81"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="86"/>
+      <c r="E42" s="86"/>
+      <c r="F42" s="86"/>
       <c r="G42" s="34"/>
       <c r="H42" s="34"/>
       <c r="I42" s="34"/>
@@ -7982,10 +10216,10 @@
     <row r="43" spans="1:11" ht="15.75" customHeight="1">
       <c r="A43" s="34"/>
       <c r="B43" s="34"/>
-      <c r="C43" s="81"/>
-      <c r="D43" s="81"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="81"/>
+      <c r="C43" s="86"/>
+      <c r="D43" s="86"/>
+      <c r="E43" s="86"/>
+      <c r="F43" s="86"/>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
       <c r="I43" s="34"/>
@@ -7995,10 +10229,10 @@
     <row r="44" spans="1:11" ht="15.75" customHeight="1">
       <c r="A44" s="34"/>
       <c r="B44" s="34"/>
-      <c r="C44" s="81"/>
-      <c r="D44" s="81"/>
-      <c r="E44" s="81"/>
-      <c r="F44" s="81"/>
+      <c r="C44" s="86"/>
+      <c r="D44" s="86"/>
+      <c r="E44" s="86"/>
+      <c r="F44" s="86"/>
       <c r="G44" s="34"/>
       <c r="H44" s="42"/>
       <c r="I44" s="34"/>
@@ -8008,10 +10242,10 @@
     <row r="45" spans="1:11" ht="13">
       <c r="A45" s="34"/>
       <c r="B45" s="34"/>
-      <c r="C45" s="81"/>
-      <c r="D45" s="81"/>
-      <c r="E45" s="81"/>
-      <c r="F45" s="81"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="86"/>
+      <c r="F45" s="86"/>
       <c r="G45" s="34"/>
       <c r="H45" s="34"/>
       <c r="I45" s="34"/>
@@ -8021,10 +10255,10 @@
     <row r="46" spans="1:11" ht="15.75" customHeight="1">
       <c r="A46" s="34"/>
       <c r="B46" s="34"/>
-      <c r="C46" s="81"/>
-      <c r="D46" s="81"/>
-      <c r="E46" s="81"/>
-      <c r="F46" s="81"/>
+      <c r="C46" s="86"/>
+      <c r="D46" s="86"/>
+      <c r="E46" s="86"/>
+      <c r="F46" s="86"/>
       <c r="G46" s="34"/>
       <c r="H46" s="34"/>
       <c r="I46" s="34"/>
@@ -8034,10 +10268,10 @@
     <row r="47" spans="1:11" ht="15.75" customHeight="1">
       <c r="A47" s="34"/>
       <c r="B47" s="34"/>
-      <c r="C47" s="81"/>
-      <c r="D47" s="81"/>
-      <c r="E47" s="81"/>
-      <c r="F47" s="81"/>
+      <c r="C47" s="86"/>
+      <c r="D47" s="86"/>
+      <c r="E47" s="86"/>
+      <c r="F47" s="86"/>
       <c r="G47" s="34"/>
       <c r="H47" s="34"/>
       <c r="I47" s="34"/>
@@ -8047,10 +10281,10 @@
     <row r="48" spans="1:11" ht="13">
       <c r="A48" s="34"/>
       <c r="B48" s="34"/>
-      <c r="C48" s="81"/>
-      <c r="D48" s="81"/>
-      <c r="E48" s="81"/>
-      <c r="F48" s="81"/>
+      <c r="C48" s="86"/>
+      <c r="D48" s="86"/>
+      <c r="E48" s="86"/>
+      <c r="F48" s="86"/>
       <c r="G48" s="34"/>
       <c r="H48" s="34"/>
       <c r="I48" s="34"/>
@@ -8060,10 +10294,10 @@
     <row r="49" spans="1:11" ht="13">
       <c r="A49" s="34"/>
       <c r="B49" s="34"/>
-      <c r="C49" s="81"/>
-      <c r="D49" s="81"/>
-      <c r="E49" s="81"/>
-      <c r="F49" s="81"/>
+      <c r="C49" s="86"/>
+      <c r="D49" s="86"/>
+      <c r="E49" s="86"/>
+      <c r="F49" s="86"/>
       <c r="G49" s="34"/>
       <c r="H49" s="34"/>
       <c r="I49" s="34"/>
@@ -8073,10 +10307,10 @@
     <row r="50" spans="1:11" ht="13">
       <c r="A50" s="34"/>
       <c r="B50" s="34"/>
-      <c r="C50" s="81"/>
-      <c r="D50" s="81"/>
-      <c r="E50" s="81"/>
-      <c r="F50" s="81"/>
+      <c r="C50" s="86"/>
+      <c r="D50" s="86"/>
+      <c r="E50" s="86"/>
+      <c r="F50" s="86"/>
       <c r="G50" s="34"/>
       <c r="H50" s="34"/>
       <c r="I50" s="34"/>
@@ -8086,10 +10320,10 @@
     <row r="51" spans="1:11" ht="13">
       <c r="A51" s="34"/>
       <c r="B51" s="34"/>
-      <c r="C51" s="81"/>
-      <c r="D51" s="81"/>
-      <c r="E51" s="81"/>
-      <c r="F51" s="81"/>
+      <c r="C51" s="86"/>
+      <c r="D51" s="86"/>
+      <c r="E51" s="86"/>
+      <c r="F51" s="86"/>
       <c r="G51" s="34"/>
       <c r="H51" s="34"/>
       <c r="I51" s="34"/>
@@ -9031,12 +11265,12 @@
     <row r="33" spans="1:11" ht="13">
       <c r="A33" s="34"/>
       <c r="B33" s="34"/>
-      <c r="C33" s="80" t="s">
+      <c r="C33" s="85" t="s">
         <v>99</v>
       </c>
-      <c r="D33" s="81"/>
-      <c r="E33" s="81"/>
-      <c r="F33" s="81"/>
+      <c r="D33" s="86"/>
+      <c r="E33" s="86"/>
+      <c r="F33" s="86"/>
       <c r="G33" s="34"/>
       <c r="H33" s="34"/>
       <c r="I33" s="34"/>
@@ -9046,10 +11280,10 @@
     <row r="34" spans="1:11" ht="13">
       <c r="A34" s="34"/>
       <c r="B34" s="34"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="81"/>
+      <c r="C34" s="86"/>
+      <c r="D34" s="86"/>
+      <c r="E34" s="86"/>
+      <c r="F34" s="86"/>
       <c r="G34" s="34"/>
       <c r="H34" s="34"/>
       <c r="I34" s="34"/>
@@ -9059,10 +11293,10 @@
     <row r="35" spans="1:11" ht="13">
       <c r="A35" s="34"/>
       <c r="B35" s="34"/>
-      <c r="C35" s="81"/>
-      <c r="D35" s="81"/>
-      <c r="E35" s="81"/>
-      <c r="F35" s="81"/>
+      <c r="C35" s="86"/>
+      <c r="D35" s="86"/>
+      <c r="E35" s="86"/>
+      <c r="F35" s="86"/>
       <c r="G35" s="34"/>
       <c r="H35" s="34"/>
       <c r="I35" s="34"/>
@@ -9072,10 +11306,10 @@
     <row r="36" spans="1:11" ht="15.75" customHeight="1">
       <c r="A36" s="34"/>
       <c r="B36" s="34"/>
-      <c r="C36" s="81"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="81"/>
-      <c r="F36" s="81"/>
+      <c r="C36" s="86"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="86"/>
+      <c r="F36" s="86"/>
       <c r="G36" s="34"/>
       <c r="H36" s="34"/>
       <c r="I36" s="34"/>
@@ -9085,10 +11319,10 @@
     <row r="37" spans="1:11" ht="15.75" customHeight="1">
       <c r="A37" s="34"/>
       <c r="B37" s="34"/>
-      <c r="C37" s="81"/>
-      <c r="D37" s="81"/>
-      <c r="E37" s="81"/>
-      <c r="F37" s="81"/>
+      <c r="C37" s="86"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="86"/>
+      <c r="F37" s="86"/>
       <c r="G37" s="34"/>
       <c r="H37" s="34"/>
       <c r="I37" s="34"/>
@@ -9098,10 +11332,10 @@
     <row r="38" spans="1:11" ht="15.75" customHeight="1">
       <c r="A38" s="34"/>
       <c r="B38" s="34"/>
-      <c r="C38" s="81"/>
-      <c r="D38" s="81"/>
-      <c r="E38" s="81"/>
-      <c r="F38" s="81"/>
+      <c r="C38" s="86"/>
+      <c r="D38" s="86"/>
+      <c r="E38" s="86"/>
+      <c r="F38" s="86"/>
       <c r="G38" s="34"/>
       <c r="H38" s="42"/>
       <c r="I38" s="34"/>
@@ -9111,10 +11345,10 @@
     <row r="39" spans="1:11" ht="13">
       <c r="A39" s="34"/>
       <c r="B39" s="34"/>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="86"/>
+      <c r="F39" s="86"/>
       <c r="G39" s="34"/>
       <c r="H39" s="34"/>
       <c r="I39" s="34"/>
@@ -9124,10 +11358,10 @@
     <row r="40" spans="1:11" ht="15.75" customHeight="1">
       <c r="A40" s="34"/>
       <c r="B40" s="34"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="81"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="86"/>
+      <c r="E40" s="86"/>
+      <c r="F40" s="86"/>
       <c r="G40" s="34"/>
       <c r="H40" s="34"/>
       <c r="I40" s="34"/>
@@ -9137,10 +11371,10 @@
     <row r="41" spans="1:11" ht="15.75" customHeight="1">
       <c r="A41" s="34"/>
       <c r="B41" s="34"/>
-      <c r="C41" s="81"/>
-      <c r="D41" s="81"/>
-      <c r="E41" s="81"/>
-      <c r="F41" s="81"/>
+      <c r="C41" s="86"/>
+      <c r="D41" s="86"/>
+      <c r="E41" s="86"/>
+      <c r="F41" s="86"/>
       <c r="G41" s="34"/>
       <c r="H41" s="34"/>
       <c r="I41" s="34"/>
@@ -9150,10 +11384,10 @@
     <row r="42" spans="1:11" ht="13">
       <c r="A42" s="34"/>
       <c r="B42" s="34"/>
-      <c r="C42" s="81"/>
-      <c r="D42" s="81"/>
-      <c r="E42" s="81"/>
-      <c r="F42" s="81"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="86"/>
+      <c r="E42" s="86"/>
+      <c r="F42" s="86"/>
       <c r="G42" s="34"/>
       <c r="H42" s="34"/>
       <c r="I42" s="34"/>
@@ -9163,10 +11397,10 @@
     <row r="43" spans="1:11" ht="13">
       <c r="A43" s="34"/>
       <c r="B43" s="34"/>
-      <c r="C43" s="81"/>
-      <c r="D43" s="81"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="81"/>
+      <c r="C43" s="86"/>
+      <c r="D43" s="86"/>
+      <c r="E43" s="86"/>
+      <c r="F43" s="86"/>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
       <c r="I43" s="34"/>
@@ -9176,10 +11410,10 @@
     <row r="44" spans="1:11" ht="13">
       <c r="A44" s="34"/>
       <c r="B44" s="34"/>
-      <c r="C44" s="81"/>
-      <c r="D44" s="81"/>
-      <c r="E44" s="81"/>
-      <c r="F44" s="81"/>
+      <c r="C44" s="86"/>
+      <c r="D44" s="86"/>
+      <c r="E44" s="86"/>
+      <c r="F44" s="86"/>
       <c r="G44" s="34"/>
       <c r="H44" s="34"/>
       <c r="I44" s="34"/>
@@ -9189,10 +11423,10 @@
     <row r="45" spans="1:11" ht="13">
       <c r="A45" s="34"/>
       <c r="B45" s="34"/>
-      <c r="C45" s="81"/>
-      <c r="D45" s="81"/>
-      <c r="E45" s="81"/>
-      <c r="F45" s="81"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="86"/>
+      <c r="F45" s="86"/>
       <c r="G45" s="34"/>
       <c r="H45" s="34"/>
       <c r="I45" s="34"/>
@@ -10094,12 +12328,12 @@
       <c r="B36" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="82" t="s">
+      <c r="C36" s="87" t="s">
         <v>185</v>
       </c>
-      <c r="D36" s="81"/>
-      <c r="E36" s="81"/>
-      <c r="F36" s="81"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="86"/>
+      <c r="F36" s="86"/>
       <c r="G36" s="34"/>
       <c r="H36" s="34"/>
       <c r="I36" s="34"/>
@@ -10109,10 +12343,10 @@
     <row r="37" spans="1:11" ht="13">
       <c r="A37" s="34"/>
       <c r="B37" s="34"/>
-      <c r="C37" s="81"/>
-      <c r="D37" s="81"/>
-      <c r="E37" s="81"/>
-      <c r="F37" s="81"/>
+      <c r="C37" s="86"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="86"/>
+      <c r="F37" s="86"/>
       <c r="G37" s="34"/>
       <c r="H37" s="34"/>
       <c r="I37" s="34"/>
@@ -10122,10 +12356,10 @@
     <row r="38" spans="1:11" ht="13">
       <c r="A38" s="34"/>
       <c r="B38" s="34"/>
-      <c r="C38" s="81"/>
-      <c r="D38" s="81"/>
-      <c r="E38" s="81"/>
-      <c r="F38" s="81"/>
+      <c r="C38" s="86"/>
+      <c r="D38" s="86"/>
+      <c r="E38" s="86"/>
+      <c r="F38" s="86"/>
       <c r="G38" s="34"/>
       <c r="H38" s="34"/>
       <c r="I38" s="34"/>
@@ -10135,10 +12369,10 @@
     <row r="39" spans="1:11" ht="15.75" customHeight="1">
       <c r="A39" s="34"/>
       <c r="B39" s="34"/>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="86"/>
+      <c r="F39" s="86"/>
       <c r="G39" s="34"/>
       <c r="H39" s="34"/>
       <c r="I39" s="34"/>
@@ -10148,10 +12382,10 @@
     <row r="40" spans="1:11" ht="15.75" customHeight="1">
       <c r="A40" s="34"/>
       <c r="B40" s="34"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="81"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="86"/>
+      <c r="E40" s="86"/>
+      <c r="F40" s="86"/>
       <c r="G40" s="34"/>
       <c r="H40" s="34"/>
       <c r="I40" s="34"/>
@@ -10161,10 +12395,10 @@
     <row r="41" spans="1:11" ht="15.75" customHeight="1">
       <c r="A41" s="34"/>
       <c r="B41" s="34"/>
-      <c r="C41" s="81"/>
-      <c r="D41" s="81"/>
-      <c r="E41" s="81"/>
-      <c r="F41" s="81"/>
+      <c r="C41" s="86"/>
+      <c r="D41" s="86"/>
+      <c r="E41" s="86"/>
+      <c r="F41" s="86"/>
       <c r="G41" s="34"/>
       <c r="H41" s="42"/>
       <c r="I41" s="34"/>
@@ -10174,10 +12408,10 @@
     <row r="42" spans="1:11" ht="13">
       <c r="A42" s="34"/>
       <c r="B42" s="34"/>
-      <c r="C42" s="81"/>
-      <c r="D42" s="81"/>
-      <c r="E42" s="81"/>
-      <c r="F42" s="81"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="86"/>
+      <c r="E42" s="86"/>
+      <c r="F42" s="86"/>
       <c r="G42" s="34"/>
       <c r="H42" s="34"/>
       <c r="I42" s="34"/>
@@ -10187,10 +12421,10 @@
     <row r="43" spans="1:11" ht="15.75" customHeight="1">
       <c r="A43" s="34"/>
       <c r="B43" s="34"/>
-      <c r="C43" s="81"/>
-      <c r="D43" s="81"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="81"/>
+      <c r="C43" s="86"/>
+      <c r="D43" s="86"/>
+      <c r="E43" s="86"/>
+      <c r="F43" s="86"/>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
       <c r="I43" s="34"/>
@@ -10200,10 +12434,10 @@
     <row r="44" spans="1:11" ht="15.75" customHeight="1">
       <c r="A44" s="34"/>
       <c r="B44" s="34"/>
-      <c r="C44" s="81"/>
-      <c r="D44" s="81"/>
-      <c r="E44" s="81"/>
-      <c r="F44" s="81"/>
+      <c r="C44" s="86"/>
+      <c r="D44" s="86"/>
+      <c r="E44" s="86"/>
+      <c r="F44" s="86"/>
       <c r="G44" s="34"/>
       <c r="H44" s="34"/>
       <c r="I44" s="34"/>
@@ -10213,10 +12447,10 @@
     <row r="45" spans="1:11" ht="13">
       <c r="A45" s="34"/>
       <c r="B45" s="34"/>
-      <c r="C45" s="81"/>
-      <c r="D45" s="81"/>
-      <c r="E45" s="81"/>
-      <c r="F45" s="81"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="86"/>
+      <c r="F45" s="86"/>
       <c r="G45" s="34"/>
       <c r="H45" s="34"/>
       <c r="I45" s="34"/>
@@ -10226,10 +12460,10 @@
     <row r="46" spans="1:11" ht="13">
       <c r="A46" s="34"/>
       <c r="B46" s="34"/>
-      <c r="C46" s="81"/>
-      <c r="D46" s="81"/>
-      <c r="E46" s="81"/>
-      <c r="F46" s="81"/>
+      <c r="C46" s="86"/>
+      <c r="D46" s="86"/>
+      <c r="E46" s="86"/>
+      <c r="F46" s="86"/>
       <c r="G46" s="34"/>
       <c r="H46" s="34"/>
       <c r="I46" s="34"/>
@@ -10239,10 +12473,10 @@
     <row r="47" spans="1:11" ht="13">
       <c r="A47" s="34"/>
       <c r="B47" s="34"/>
-      <c r="C47" s="81"/>
-      <c r="D47" s="81"/>
-      <c r="E47" s="81"/>
-      <c r="F47" s="81"/>
+      <c r="C47" s="86"/>
+      <c r="D47" s="86"/>
+      <c r="E47" s="86"/>
+      <c r="F47" s="86"/>
       <c r="G47" s="34"/>
       <c r="H47" s="34"/>
       <c r="I47" s="34"/>
@@ -10252,10 +12486,10 @@
     <row r="48" spans="1:11" ht="13">
       <c r="A48" s="34"/>
       <c r="B48" s="34"/>
-      <c r="C48" s="81"/>
-      <c r="D48" s="81"/>
-      <c r="E48" s="81"/>
-      <c r="F48" s="81"/>
+      <c r="C48" s="86"/>
+      <c r="D48" s="86"/>
+      <c r="E48" s="86"/>
+      <c r="F48" s="86"/>
       <c r="G48" s="34"/>
       <c r="H48" s="34"/>
       <c r="I48" s="34"/>
@@ -11016,12 +13250,12 @@
     <row r="34" spans="1:11" ht="13">
       <c r="A34" s="34"/>
       <c r="B34" s="34"/>
-      <c r="C34" s="80" t="s">
+      <c r="C34" s="85" t="s">
         <v>123</v>
       </c>
-      <c r="D34" s="81"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="81"/>
+      <c r="D34" s="86"/>
+      <c r="E34" s="86"/>
+      <c r="F34" s="86"/>
       <c r="G34" s="34"/>
       <c r="H34" s="34"/>
       <c r="I34" s="34"/>
@@ -11031,10 +13265,10 @@
     <row r="35" spans="1:11" ht="13">
       <c r="A35" s="34"/>
       <c r="B35" s="34"/>
-      <c r="C35" s="81"/>
-      <c r="D35" s="81"/>
-      <c r="E35" s="81"/>
-      <c r="F35" s="81"/>
+      <c r="C35" s="86"/>
+      <c r="D35" s="86"/>
+      <c r="E35" s="86"/>
+      <c r="F35" s="86"/>
       <c r="G35" s="34"/>
       <c r="H35" s="34"/>
       <c r="I35" s="34"/>
@@ -11044,10 +13278,10 @@
     <row r="36" spans="1:11" ht="13">
       <c r="A36" s="34"/>
       <c r="B36" s="34"/>
-      <c r="C36" s="81"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="81"/>
-      <c r="F36" s="81"/>
+      <c r="C36" s="86"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="86"/>
+      <c r="F36" s="86"/>
       <c r="G36" s="34"/>
       <c r="H36" s="34"/>
       <c r="I36" s="34"/>
@@ -11057,10 +13291,10 @@
     <row r="37" spans="1:11" ht="15.75" customHeight="1">
       <c r="A37" s="34"/>
       <c r="B37" s="34"/>
-      <c r="C37" s="81"/>
-      <c r="D37" s="81"/>
-      <c r="E37" s="81"/>
-      <c r="F37" s="81"/>
+      <c r="C37" s="86"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="86"/>
+      <c r="F37" s="86"/>
       <c r="G37" s="34"/>
       <c r="H37" s="34"/>
       <c r="I37" s="34"/>
@@ -11070,10 +13304,10 @@
     <row r="38" spans="1:11" ht="15.75" customHeight="1">
       <c r="A38" s="34"/>
       <c r="B38" s="34"/>
-      <c r="C38" s="81"/>
-      <c r="D38" s="81"/>
-      <c r="E38" s="81"/>
-      <c r="F38" s="81"/>
+      <c r="C38" s="86"/>
+      <c r="D38" s="86"/>
+      <c r="E38" s="86"/>
+      <c r="F38" s="86"/>
       <c r="G38" s="34"/>
       <c r="H38" s="34"/>
       <c r="I38" s="34"/>
@@ -11083,10 +13317,10 @@
     <row r="39" spans="1:11" ht="15.75" customHeight="1">
       <c r="A39" s="34"/>
       <c r="B39" s="34"/>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="86"/>
+      <c r="F39" s="86"/>
       <c r="G39" s="34"/>
       <c r="H39" s="42"/>
       <c r="I39" s="34"/>
@@ -11096,10 +13330,10 @@
     <row r="40" spans="1:11" ht="13">
       <c r="A40" s="34"/>
       <c r="B40" s="34"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="81"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="86"/>
+      <c r="E40" s="86"/>
+      <c r="F40" s="86"/>
       <c r="G40" s="34"/>
       <c r="H40" s="34"/>
       <c r="I40" s="34"/>
@@ -11109,10 +13343,10 @@
     <row r="41" spans="1:11" ht="15.75" customHeight="1">
       <c r="A41" s="34"/>
       <c r="B41" s="34"/>
-      <c r="C41" s="81"/>
-      <c r="D41" s="81"/>
-      <c r="E41" s="81"/>
-      <c r="F41" s="81"/>
+      <c r="C41" s="86"/>
+      <c r="D41" s="86"/>
+      <c r="E41" s="86"/>
+      <c r="F41" s="86"/>
       <c r="G41" s="34"/>
       <c r="H41" s="34"/>
       <c r="I41" s="34"/>
@@ -11122,10 +13356,10 @@
     <row r="42" spans="1:11" ht="15.75" customHeight="1">
       <c r="A42" s="34"/>
       <c r="B42" s="34"/>
-      <c r="C42" s="81"/>
-      <c r="D42" s="81"/>
-      <c r="E42" s="81"/>
-      <c r="F42" s="81"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="86"/>
+      <c r="E42" s="86"/>
+      <c r="F42" s="86"/>
       <c r="G42" s="34"/>
       <c r="H42" s="34"/>
       <c r="I42" s="34"/>
@@ -11135,10 +13369,10 @@
     <row r="43" spans="1:11" ht="13">
       <c r="A43" s="34"/>
       <c r="B43" s="34"/>
-      <c r="C43" s="81"/>
-      <c r="D43" s="81"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="81"/>
+      <c r="C43" s="86"/>
+      <c r="D43" s="86"/>
+      <c r="E43" s="86"/>
+      <c r="F43" s="86"/>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
       <c r="I43" s="34"/>
@@ -11148,10 +13382,10 @@
     <row r="44" spans="1:11" ht="13">
       <c r="A44" s="34"/>
       <c r="B44" s="34"/>
-      <c r="C44" s="81"/>
-      <c r="D44" s="81"/>
-      <c r="E44" s="81"/>
-      <c r="F44" s="81"/>
+      <c r="C44" s="86"/>
+      <c r="D44" s="86"/>
+      <c r="E44" s="86"/>
+      <c r="F44" s="86"/>
       <c r="G44" s="34"/>
       <c r="H44" s="34"/>
       <c r="I44" s="34"/>
@@ -11161,10 +13395,10 @@
     <row r="45" spans="1:11" ht="13">
       <c r="A45" s="34"/>
       <c r="B45" s="34"/>
-      <c r="C45" s="81"/>
-      <c r="D45" s="81"/>
-      <c r="E45" s="81"/>
-      <c r="F45" s="81"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="86"/>
+      <c r="F45" s="86"/>
       <c r="G45" s="34"/>
       <c r="H45" s="34"/>
       <c r="I45" s="34"/>
@@ -11174,10 +13408,10 @@
     <row r="46" spans="1:11" ht="13">
       <c r="A46" s="34"/>
       <c r="B46" s="34"/>
-      <c r="C46" s="81"/>
-      <c r="D46" s="81"/>
-      <c r="E46" s="81"/>
-      <c r="F46" s="81"/>
+      <c r="C46" s="86"/>
+      <c r="D46" s="86"/>
+      <c r="E46" s="86"/>
+      <c r="F46" s="86"/>
       <c r="G46" s="34"/>
       <c r="H46" s="34"/>
       <c r="I46" s="34"/>
@@ -11423,7 +13657,7 @@
   <dimension ref="A1:K103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection sqref="A1:H94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -12284,12 +14518,12 @@
     <row r="48" spans="1:11" ht="13">
       <c r="A48" s="34"/>
       <c r="B48" s="34"/>
-      <c r="C48" s="80" t="s">
+      <c r="C48" s="85" t="s">
         <v>152</v>
       </c>
-      <c r="D48" s="81"/>
-      <c r="E48" s="81"/>
-      <c r="F48" s="81"/>
+      <c r="D48" s="86"/>
+      <c r="E48" s="86"/>
+      <c r="F48" s="86"/>
       <c r="G48" s="34"/>
       <c r="H48" s="34"/>
       <c r="I48" s="34"/>
@@ -12299,10 +14533,10 @@
     <row r="49" spans="1:11" ht="13">
       <c r="A49" s="34"/>
       <c r="B49" s="34"/>
-      <c r="C49" s="81"/>
-      <c r="D49" s="81"/>
-      <c r="E49" s="81"/>
-      <c r="F49" s="81"/>
+      <c r="C49" s="86"/>
+      <c r="D49" s="86"/>
+      <c r="E49" s="86"/>
+      <c r="F49" s="86"/>
       <c r="G49" s="34"/>
       <c r="H49" s="34"/>
       <c r="I49" s="34"/>
@@ -12312,10 +14546,10 @@
     <row r="50" spans="1:11" ht="13">
       <c r="A50" s="34"/>
       <c r="B50" s="34"/>
-      <c r="C50" s="81"/>
-      <c r="D50" s="81"/>
-      <c r="E50" s="81"/>
-      <c r="F50" s="81"/>
+      <c r="C50" s="86"/>
+      <c r="D50" s="86"/>
+      <c r="E50" s="86"/>
+      <c r="F50" s="86"/>
       <c r="G50" s="34"/>
       <c r="H50" s="34"/>
       <c r="I50" s="34"/>
@@ -12325,10 +14559,10 @@
     <row r="51" spans="1:11" ht="15.75" customHeight="1">
       <c r="A51" s="34"/>
       <c r="B51" s="34"/>
-      <c r="C51" s="81"/>
-      <c r="D51" s="81"/>
-      <c r="E51" s="81"/>
-      <c r="F51" s="81"/>
+      <c r="C51" s="86"/>
+      <c r="D51" s="86"/>
+      <c r="E51" s="86"/>
+      <c r="F51" s="86"/>
       <c r="G51" s="34"/>
       <c r="H51" s="34"/>
       <c r="I51" s="34"/>
@@ -12338,10 +14572,10 @@
     <row r="52" spans="1:11" ht="15.75" customHeight="1">
       <c r="A52" s="34"/>
       <c r="B52" s="34"/>
-      <c r="C52" s="81"/>
-      <c r="D52" s="81"/>
-      <c r="E52" s="81"/>
-      <c r="F52" s="81"/>
+      <c r="C52" s="86"/>
+      <c r="D52" s="86"/>
+      <c r="E52" s="86"/>
+      <c r="F52" s="86"/>
       <c r="G52" s="34"/>
       <c r="H52" s="34"/>
       <c r="I52" s="34"/>
@@ -12351,10 +14585,10 @@
     <row r="53" spans="1:11" ht="15.75" customHeight="1">
       <c r="A53" s="34"/>
       <c r="B53" s="34"/>
-      <c r="C53" s="81"/>
-      <c r="D53" s="81"/>
-      <c r="E53" s="81"/>
-      <c r="F53" s="81"/>
+      <c r="C53" s="86"/>
+      <c r="D53" s="86"/>
+      <c r="E53" s="86"/>
+      <c r="F53" s="86"/>
       <c r="G53" s="34"/>
       <c r="H53" s="42"/>
       <c r="I53" s="34"/>
@@ -12364,10 +14598,10 @@
     <row r="54" spans="1:11" ht="13">
       <c r="A54" s="34"/>
       <c r="B54" s="34"/>
-      <c r="C54" s="81"/>
-      <c r="D54" s="81"/>
-      <c r="E54" s="81"/>
-      <c r="F54" s="81"/>
+      <c r="C54" s="86"/>
+      <c r="D54" s="86"/>
+      <c r="E54" s="86"/>
+      <c r="F54" s="86"/>
       <c r="G54" s="34"/>
       <c r="H54" s="34"/>
       <c r="I54" s="34"/>
@@ -12377,10 +14611,10 @@
     <row r="55" spans="1:11" ht="15.75" customHeight="1">
       <c r="A55" s="34"/>
       <c r="B55" s="34"/>
-      <c r="C55" s="81"/>
-      <c r="D55" s="81"/>
-      <c r="E55" s="81"/>
-      <c r="F55" s="81"/>
+      <c r="C55" s="86"/>
+      <c r="D55" s="86"/>
+      <c r="E55" s="86"/>
+      <c r="F55" s="86"/>
       <c r="G55" s="34"/>
       <c r="H55" s="34"/>
       <c r="I55" s="34"/>
@@ -12390,10 +14624,10 @@
     <row r="56" spans="1:11" ht="15.75" customHeight="1">
       <c r="A56" s="34"/>
       <c r="B56" s="34"/>
-      <c r="C56" s="81"/>
-      <c r="D56" s="81"/>
-      <c r="E56" s="81"/>
-      <c r="F56" s="81"/>
+      <c r="C56" s="86"/>
+      <c r="D56" s="86"/>
+      <c r="E56" s="86"/>
+      <c r="F56" s="86"/>
       <c r="G56" s="34"/>
       <c r="H56" s="34"/>
       <c r="I56" s="34"/>
@@ -12403,10 +14637,10 @@
     <row r="57" spans="1:11" ht="13">
       <c r="A57" s="34"/>
       <c r="B57" s="34"/>
-      <c r="C57" s="81"/>
-      <c r="D57" s="81"/>
-      <c r="E57" s="81"/>
-      <c r="F57" s="81"/>
+      <c r="C57" s="86"/>
+      <c r="D57" s="86"/>
+      <c r="E57" s="86"/>
+      <c r="F57" s="86"/>
       <c r="G57" s="34"/>
       <c r="H57" s="34"/>
       <c r="I57" s="34"/>
@@ -12416,10 +14650,10 @@
     <row r="58" spans="1:11" ht="13">
       <c r="A58" s="34"/>
       <c r="B58" s="34"/>
-      <c r="C58" s="81"/>
-      <c r="D58" s="81"/>
-      <c r="E58" s="81"/>
-      <c r="F58" s="81"/>
+      <c r="C58" s="86"/>
+      <c r="D58" s="86"/>
+      <c r="E58" s="86"/>
+      <c r="F58" s="86"/>
       <c r="G58" s="34"/>
       <c r="H58" s="34"/>
       <c r="I58" s="34"/>
@@ -12429,10 +14663,10 @@
     <row r="59" spans="1:11" ht="13">
       <c r="A59" s="34"/>
       <c r="B59" s="34"/>
-      <c r="C59" s="81"/>
-      <c r="D59" s="81"/>
-      <c r="E59" s="81"/>
-      <c r="F59" s="81"/>
+      <c r="C59" s="86"/>
+      <c r="D59" s="86"/>
+      <c r="E59" s="86"/>
+      <c r="F59" s="86"/>
       <c r="G59" s="34"/>
       <c r="H59" s="34"/>
       <c r="I59" s="34"/>
@@ -12442,10 +14676,10 @@
     <row r="60" spans="1:11" ht="13">
       <c r="A60" s="34"/>
       <c r="B60" s="34"/>
-      <c r="C60" s="81"/>
-      <c r="D60" s="81"/>
-      <c r="E60" s="81"/>
-      <c r="F60" s="81"/>
+      <c r="C60" s="86"/>
+      <c r="D60" s="86"/>
+      <c r="E60" s="86"/>
+      <c r="F60" s="86"/>
       <c r="G60" s="34"/>
       <c r="H60" s="34"/>
       <c r="I60" s="34"/>
@@ -12455,10 +14689,10 @@
     <row r="61" spans="1:11" ht="13">
       <c r="A61" s="34"/>
       <c r="B61" s="34"/>
-      <c r="C61" s="81"/>
-      <c r="D61" s="81"/>
-      <c r="E61" s="81"/>
-      <c r="F61" s="81"/>
+      <c r="C61" s="86"/>
+      <c r="D61" s="86"/>
+      <c r="E61" s="86"/>
+      <c r="F61" s="86"/>
       <c r="G61" s="34"/>
       <c r="H61" s="34"/>
       <c r="I61" s="34"/>
@@ -12468,10 +14702,10 @@
     <row r="62" spans="1:11" ht="13">
       <c r="A62" s="34"/>
       <c r="B62" s="34"/>
-      <c r="C62" s="81"/>
-      <c r="D62" s="81"/>
-      <c r="E62" s="81"/>
-      <c r="F62" s="81"/>
+      <c r="C62" s="86"/>
+      <c r="D62" s="86"/>
+      <c r="E62" s="86"/>
+      <c r="F62" s="86"/>
       <c r="G62" s="34"/>
       <c r="H62" s="34"/>
       <c r="I62" s="34"/>
@@ -12481,10 +14715,10 @@
     <row r="63" spans="1:11" ht="13">
       <c r="A63" s="34"/>
       <c r="B63" s="34"/>
-      <c r="C63" s="81"/>
-      <c r="D63" s="81"/>
-      <c r="E63" s="81"/>
-      <c r="F63" s="81"/>
+      <c r="C63" s="86"/>
+      <c r="D63" s="86"/>
+      <c r="E63" s="86"/>
+      <c r="F63" s="86"/>
       <c r="G63" s="34"/>
       <c r="H63" s="34"/>
       <c r="I63" s="34"/>
@@ -12494,10 +14728,10 @@
     <row r="64" spans="1:11" ht="13">
       <c r="A64" s="34"/>
       <c r="B64" s="34"/>
-      <c r="C64" s="81"/>
-      <c r="D64" s="81"/>
-      <c r="E64" s="81"/>
-      <c r="F64" s="81"/>
+      <c r="C64" s="86"/>
+      <c r="D64" s="86"/>
+      <c r="E64" s="86"/>
+      <c r="F64" s="86"/>
       <c r="G64" s="34"/>
       <c r="H64" s="34"/>
       <c r="I64" s="34"/>
@@ -12507,10 +14741,10 @@
     <row r="65" spans="1:11" ht="13">
       <c r="A65" s="34"/>
       <c r="B65" s="34"/>
-      <c r="C65" s="81"/>
-      <c r="D65" s="81"/>
-      <c r="E65" s="81"/>
-      <c r="F65" s="81"/>
+      <c r="C65" s="86"/>
+      <c r="D65" s="86"/>
+      <c r="E65" s="86"/>
+      <c r="F65" s="86"/>
       <c r="G65" s="34"/>
       <c r="H65" s="34"/>
       <c r="I65" s="34"/>
@@ -12520,10 +14754,10 @@
     <row r="66" spans="1:11" ht="13">
       <c r="A66" s="34"/>
       <c r="B66" s="34"/>
-      <c r="C66" s="81"/>
-      <c r="D66" s="81"/>
-      <c r="E66" s="81"/>
-      <c r="F66" s="81"/>
+      <c r="C66" s="86"/>
+      <c r="D66" s="86"/>
+      <c r="E66" s="86"/>
+      <c r="F66" s="86"/>
       <c r="G66" s="34"/>
       <c r="H66" s="34"/>
       <c r="I66" s="34"/>
@@ -12533,10 +14767,10 @@
     <row r="67" spans="1:11" ht="13">
       <c r="A67" s="34"/>
       <c r="B67" s="34"/>
-      <c r="C67" s="81"/>
-      <c r="D67" s="81"/>
-      <c r="E67" s="81"/>
-      <c r="F67" s="81"/>
+      <c r="C67" s="86"/>
+      <c r="D67" s="86"/>
+      <c r="E67" s="86"/>
+      <c r="F67" s="86"/>
       <c r="G67" s="34"/>
       <c r="H67" s="34"/>
       <c r="I67" s="34"/>
@@ -12546,10 +14780,10 @@
     <row r="68" spans="1:11" ht="13">
       <c r="A68" s="34"/>
       <c r="B68" s="34"/>
-      <c r="C68" s="81"/>
-      <c r="D68" s="81"/>
-      <c r="E68" s="81"/>
-      <c r="F68" s="81"/>
+      <c r="C68" s="86"/>
+      <c r="D68" s="86"/>
+      <c r="E68" s="86"/>
+      <c r="F68" s="86"/>
       <c r="G68" s="34"/>
       <c r="H68" s="34"/>
       <c r="I68" s="34"/>
@@ -12559,10 +14793,10 @@
     <row r="69" spans="1:11" ht="13">
       <c r="A69" s="34"/>
       <c r="B69" s="34"/>
-      <c r="C69" s="81"/>
-      <c r="D69" s="81"/>
-      <c r="E69" s="81"/>
-      <c r="F69" s="81"/>
+      <c r="C69" s="86"/>
+      <c r="D69" s="86"/>
+      <c r="E69" s="86"/>
+      <c r="F69" s="86"/>
       <c r="G69" s="34"/>
       <c r="H69" s="34"/>
       <c r="I69" s="34"/>
@@ -12572,10 +14806,10 @@
     <row r="70" spans="1:11" ht="13">
       <c r="A70" s="34"/>
       <c r="B70" s="34"/>
-      <c r="C70" s="81"/>
-      <c r="D70" s="81"/>
-      <c r="E70" s="81"/>
-      <c r="F70" s="81"/>
+      <c r="C70" s="86"/>
+      <c r="D70" s="86"/>
+      <c r="E70" s="86"/>
+      <c r="F70" s="86"/>
       <c r="G70" s="34"/>
       <c r="H70" s="34"/>
       <c r="I70" s="34"/>
@@ -12585,10 +14819,10 @@
     <row r="71" spans="1:11" ht="13">
       <c r="A71" s="34"/>
       <c r="B71" s="34"/>
-      <c r="C71" s="81"/>
-      <c r="D71" s="81"/>
-      <c r="E71" s="81"/>
-      <c r="F71" s="81"/>
+      <c r="C71" s="86"/>
+      <c r="D71" s="86"/>
+      <c r="E71" s="86"/>
+      <c r="F71" s="86"/>
       <c r="G71" s="34"/>
       <c r="H71" s="34"/>
       <c r="I71" s="34"/>
@@ -12598,10 +14832,10 @@
     <row r="72" spans="1:11" ht="13">
       <c r="A72" s="34"/>
       <c r="B72" s="34"/>
-      <c r="C72" s="81"/>
-      <c r="D72" s="81"/>
-      <c r="E72" s="81"/>
-      <c r="F72" s="81"/>
+      <c r="C72" s="86"/>
+      <c r="D72" s="86"/>
+      <c r="E72" s="86"/>
+      <c r="F72" s="86"/>
       <c r="G72" s="34"/>
       <c r="H72" s="34"/>
       <c r="I72" s="34"/>
@@ -12611,10 +14845,10 @@
     <row r="73" spans="1:11" ht="13">
       <c r="A73" s="34"/>
       <c r="B73" s="34"/>
-      <c r="C73" s="81"/>
-      <c r="D73" s="81"/>
-      <c r="E73" s="81"/>
-      <c r="F73" s="81"/>
+      <c r="C73" s="86"/>
+      <c r="D73" s="86"/>
+      <c r="E73" s="86"/>
+      <c r="F73" s="86"/>
       <c r="G73" s="34"/>
       <c r="H73" s="34"/>
       <c r="I73" s="34"/>
@@ -12624,10 +14858,10 @@
     <row r="74" spans="1:11" ht="13">
       <c r="A74" s="34"/>
       <c r="B74" s="34"/>
-      <c r="C74" s="81"/>
-      <c r="D74" s="81"/>
-      <c r="E74" s="81"/>
-      <c r="F74" s="81"/>
+      <c r="C74" s="86"/>
+      <c r="D74" s="86"/>
+      <c r="E74" s="86"/>
+      <c r="F74" s="86"/>
       <c r="G74" s="34"/>
       <c r="H74" s="34"/>
       <c r="I74" s="34"/>
@@ -12637,10 +14871,10 @@
     <row r="75" spans="1:11" ht="13">
       <c r="A75" s="34"/>
       <c r="B75" s="34"/>
-      <c r="C75" s="81"/>
-      <c r="D75" s="81"/>
-      <c r="E75" s="81"/>
-      <c r="F75" s="81"/>
+      <c r="C75" s="86"/>
+      <c r="D75" s="86"/>
+      <c r="E75" s="86"/>
+      <c r="F75" s="86"/>
       <c r="G75" s="34"/>
       <c r="H75" s="34"/>
       <c r="I75" s="34"/>
@@ -12650,10 +14884,10 @@
     <row r="76" spans="1:11" ht="13">
       <c r="A76" s="34"/>
       <c r="B76" s="34"/>
-      <c r="C76" s="81"/>
-      <c r="D76" s="81"/>
-      <c r="E76" s="81"/>
-      <c r="F76" s="81"/>
+      <c r="C76" s="86"/>
+      <c r="D76" s="86"/>
+      <c r="E76" s="86"/>
+      <c r="F76" s="86"/>
       <c r="G76" s="34"/>
       <c r="H76" s="34"/>
       <c r="I76" s="34"/>
@@ -12663,10 +14897,10 @@
     <row r="77" spans="1:11" ht="13">
       <c r="A77" s="34"/>
       <c r="B77" s="34"/>
-      <c r="C77" s="81"/>
-      <c r="D77" s="81"/>
-      <c r="E77" s="81"/>
-      <c r="F77" s="81"/>
+      <c r="C77" s="86"/>
+      <c r="D77" s="86"/>
+      <c r="E77" s="86"/>
+      <c r="F77" s="86"/>
       <c r="G77" s="34"/>
       <c r="H77" s="34"/>
       <c r="I77" s="34"/>
@@ -12676,10 +14910,10 @@
     <row r="78" spans="1:11" ht="13">
       <c r="A78" s="34"/>
       <c r="B78" s="34"/>
-      <c r="C78" s="81"/>
-      <c r="D78" s="81"/>
-      <c r="E78" s="81"/>
-      <c r="F78" s="81"/>
+      <c r="C78" s="86"/>
+      <c r="D78" s="86"/>
+      <c r="E78" s="86"/>
+      <c r="F78" s="86"/>
       <c r="G78" s="34"/>
       <c r="H78" s="34"/>
       <c r="I78" s="34"/>
@@ -12689,10 +14923,10 @@
     <row r="79" spans="1:11" ht="13">
       <c r="A79" s="34"/>
       <c r="B79" s="34"/>
-      <c r="C79" s="81"/>
-      <c r="D79" s="81"/>
-      <c r="E79" s="81"/>
-      <c r="F79" s="81"/>
+      <c r="C79" s="86"/>
+      <c r="D79" s="86"/>
+      <c r="E79" s="86"/>
+      <c r="F79" s="86"/>
       <c r="G79" s="34"/>
       <c r="H79" s="34"/>
       <c r="I79" s="34"/>
@@ -12702,10 +14936,10 @@
     <row r="80" spans="1:11" ht="13">
       <c r="A80" s="34"/>
       <c r="B80" s="34"/>
-      <c r="C80" s="81"/>
-      <c r="D80" s="81"/>
-      <c r="E80" s="81"/>
-      <c r="F80" s="81"/>
+      <c r="C80" s="86"/>
+      <c r="D80" s="86"/>
+      <c r="E80" s="86"/>
+      <c r="F80" s="86"/>
       <c r="G80" s="34"/>
       <c r="H80" s="34"/>
       <c r="I80" s="34"/>
@@ -12715,10 +14949,10 @@
     <row r="81" spans="1:11" ht="13">
       <c r="A81" s="34"/>
       <c r="B81" s="34"/>
-      <c r="C81" s="81"/>
-      <c r="D81" s="81"/>
-      <c r="E81" s="81"/>
-      <c r="F81" s="81"/>
+      <c r="C81" s="86"/>
+      <c r="D81" s="86"/>
+      <c r="E81" s="86"/>
+      <c r="F81" s="86"/>
       <c r="G81" s="34"/>
       <c r="H81" s="34"/>
       <c r="I81" s="34"/>
@@ -12728,10 +14962,10 @@
     <row r="82" spans="1:11" ht="13">
       <c r="A82" s="34"/>
       <c r="B82" s="34"/>
-      <c r="C82" s="81"/>
-      <c r="D82" s="81"/>
-      <c r="E82" s="81"/>
-      <c r="F82" s="81"/>
+      <c r="C82" s="86"/>
+      <c r="D82" s="86"/>
+      <c r="E82" s="86"/>
+      <c r="F82" s="86"/>
       <c r="G82" s="34"/>
       <c r="H82" s="34"/>
       <c r="I82" s="34"/>
@@ -12741,10 +14975,10 @@
     <row r="83" spans="1:11" ht="13">
       <c r="A83" s="34"/>
       <c r="B83" s="34"/>
-      <c r="C83" s="81"/>
-      <c r="D83" s="81"/>
-      <c r="E83" s="81"/>
-      <c r="F83" s="81"/>
+      <c r="C83" s="86"/>
+      <c r="D83" s="86"/>
+      <c r="E83" s="86"/>
+      <c r="F83" s="86"/>
       <c r="G83" s="34"/>
       <c r="H83" s="34"/>
       <c r="I83" s="34"/>
@@ -12754,10 +14988,10 @@
     <row r="84" spans="1:11" ht="13">
       <c r="A84" s="34"/>
       <c r="B84" s="34"/>
-      <c r="C84" s="81"/>
-      <c r="D84" s="81"/>
-      <c r="E84" s="81"/>
-      <c r="F84" s="81"/>
+      <c r="C84" s="86"/>
+      <c r="D84" s="86"/>
+      <c r="E84" s="86"/>
+      <c r="F84" s="86"/>
       <c r="G84" s="34"/>
       <c r="H84" s="34"/>
       <c r="I84" s="34"/>
@@ -12767,10 +15001,10 @@
     <row r="85" spans="1:11" ht="13">
       <c r="A85" s="34"/>
       <c r="B85" s="34"/>
-      <c r="C85" s="81"/>
-      <c r="D85" s="81"/>
-      <c r="E85" s="81"/>
-      <c r="F85" s="81"/>
+      <c r="C85" s="86"/>
+      <c r="D85" s="86"/>
+      <c r="E85" s="86"/>
+      <c r="F85" s="86"/>
       <c r="G85" s="34"/>
       <c r="H85" s="34"/>
       <c r="I85" s="34"/>
@@ -12780,10 +15014,10 @@
     <row r="86" spans="1:11" ht="13">
       <c r="A86" s="34"/>
       <c r="B86" s="34"/>
-      <c r="C86" s="81"/>
-      <c r="D86" s="81"/>
-      <c r="E86" s="81"/>
-      <c r="F86" s="81"/>
+      <c r="C86" s="86"/>
+      <c r="D86" s="86"/>
+      <c r="E86" s="86"/>
+      <c r="F86" s="86"/>
       <c r="G86" s="34"/>
       <c r="H86" s="34"/>
       <c r="I86" s="34"/>
@@ -13056,7 +15290,9 @@
   </sheetPr>
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -13383,22 +15619,12 @@
     <row r="19" spans="1:11" ht="13">
       <c r="A19" s="34"/>
       <c r="B19" s="34"/>
-      <c r="C19" s="57" t="s">
-        <v>113</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="48">
-        <v>3</v>
-      </c>
+      <c r="C19" s="57"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="48"/>
       <c r="G19" s="27"/>
-      <c r="H19" s="63" t="s">
-        <v>127</v>
-      </c>
+      <c r="H19" s="63"/>
       <c r="I19" s="27"/>
       <c r="J19" s="34"/>
       <c r="K19" s="35"/>
@@ -13661,12 +15887,12 @@
     <row r="35" spans="1:11" ht="13">
       <c r="A35" s="34"/>
       <c r="B35" s="34"/>
-      <c r="C35" s="80" t="s">
-        <v>160</v>
-      </c>
-      <c r="D35" s="81"/>
-      <c r="E35" s="81"/>
-      <c r="F35" s="81"/>
+      <c r="C35" s="87" t="s">
+        <v>213</v>
+      </c>
+      <c r="D35" s="86"/>
+      <c r="E35" s="86"/>
+      <c r="F35" s="86"/>
       <c r="G35" s="34"/>
       <c r="H35" s="34"/>
       <c r="I35" s="34"/>
@@ -13676,10 +15902,10 @@
     <row r="36" spans="1:11" ht="13">
       <c r="A36" s="34"/>
       <c r="B36" s="34"/>
-      <c r="C36" s="81"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="81"/>
-      <c r="F36" s="81"/>
+      <c r="C36" s="86"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="86"/>
+      <c r="F36" s="86"/>
       <c r="G36" s="34"/>
       <c r="H36" s="34"/>
       <c r="I36" s="34"/>
@@ -13689,10 +15915,10 @@
     <row r="37" spans="1:11" ht="13">
       <c r="A37" s="34"/>
       <c r="B37" s="34"/>
-      <c r="C37" s="81"/>
-      <c r="D37" s="81"/>
-      <c r="E37" s="81"/>
-      <c r="F37" s="81"/>
+      <c r="C37" s="86"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="86"/>
+      <c r="F37" s="86"/>
       <c r="G37" s="34"/>
       <c r="H37" s="34"/>
       <c r="I37" s="34"/>
@@ -13702,10 +15928,10 @@
     <row r="38" spans="1:11" ht="15.75" customHeight="1">
       <c r="A38" s="34"/>
       <c r="B38" s="34"/>
-      <c r="C38" s="81"/>
-      <c r="D38" s="81"/>
-      <c r="E38" s="81"/>
-      <c r="F38" s="81"/>
+      <c r="C38" s="86"/>
+      <c r="D38" s="86"/>
+      <c r="E38" s="86"/>
+      <c r="F38" s="86"/>
       <c r="G38" s="34"/>
       <c r="H38" s="34"/>
       <c r="I38" s="34"/>
@@ -13715,10 +15941,10 @@
     <row r="39" spans="1:11" ht="15.75" customHeight="1">
       <c r="A39" s="34"/>
       <c r="B39" s="34"/>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="86"/>
+      <c r="F39" s="86"/>
       <c r="G39" s="34"/>
       <c r="H39" s="34"/>
       <c r="I39" s="34"/>
@@ -13728,10 +15954,10 @@
     <row r="40" spans="1:11" ht="15.75" customHeight="1">
       <c r="A40" s="34"/>
       <c r="B40" s="34"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="81"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="86"/>
+      <c r="E40" s="86"/>
+      <c r="F40" s="86"/>
       <c r="G40" s="34"/>
       <c r="H40" s="42"/>
       <c r="I40" s="34"/>
@@ -13741,10 +15967,10 @@
     <row r="41" spans="1:11" ht="13">
       <c r="A41" s="34"/>
       <c r="B41" s="34"/>
-      <c r="C41" s="81"/>
-      <c r="D41" s="81"/>
-      <c r="E41" s="81"/>
-      <c r="F41" s="81"/>
+      <c r="C41" s="86"/>
+      <c r="D41" s="86"/>
+      <c r="E41" s="86"/>
+      <c r="F41" s="86"/>
       <c r="G41" s="34"/>
       <c r="H41" s="34"/>
       <c r="I41" s="34"/>
@@ -13754,10 +15980,10 @@
     <row r="42" spans="1:11" ht="15.75" customHeight="1">
       <c r="A42" s="34"/>
       <c r="B42" s="34"/>
-      <c r="C42" s="81"/>
-      <c r="D42" s="81"/>
-      <c r="E42" s="81"/>
-      <c r="F42" s="81"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="86"/>
+      <c r="E42" s="86"/>
+      <c r="F42" s="86"/>
       <c r="G42" s="34"/>
       <c r="H42" s="34"/>
       <c r="I42" s="34"/>
@@ -13767,10 +15993,10 @@
     <row r="43" spans="1:11" ht="15.75" customHeight="1">
       <c r="A43" s="34"/>
       <c r="B43" s="34"/>
-      <c r="C43" s="81"/>
-      <c r="D43" s="81"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="81"/>
+      <c r="C43" s="86"/>
+      <c r="D43" s="86"/>
+      <c r="E43" s="86"/>
+      <c r="F43" s="86"/>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
       <c r="I43" s="34"/>
@@ -13780,10 +16006,10 @@
     <row r="44" spans="1:11" ht="13">
       <c r="A44" s="34"/>
       <c r="B44" s="34"/>
-      <c r="C44" s="81"/>
-      <c r="D44" s="81"/>
-      <c r="E44" s="81"/>
-      <c r="F44" s="81"/>
+      <c r="C44" s="86"/>
+      <c r="D44" s="86"/>
+      <c r="E44" s="86"/>
+      <c r="F44" s="86"/>
       <c r="G44" s="34"/>
       <c r="H44" s="34"/>
       <c r="I44" s="34"/>
@@ -13793,10 +16019,10 @@
     <row r="45" spans="1:11" ht="13">
       <c r="A45" s="34"/>
       <c r="B45" s="34"/>
-      <c r="C45" s="81"/>
-      <c r="D45" s="81"/>
-      <c r="E45" s="81"/>
-      <c r="F45" s="81"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="86"/>
+      <c r="F45" s="86"/>
       <c r="G45" s="34"/>
       <c r="H45" s="34"/>
       <c r="I45" s="34"/>
@@ -13806,10 +16032,10 @@
     <row r="46" spans="1:11" ht="13">
       <c r="A46" s="34"/>
       <c r="B46" s="34"/>
-      <c r="C46" s="81"/>
-      <c r="D46" s="81"/>
-      <c r="E46" s="81"/>
-      <c r="F46" s="81"/>
+      <c r="C46" s="86"/>
+      <c r="D46" s="86"/>
+      <c r="E46" s="86"/>
+      <c r="F46" s="86"/>
       <c r="G46" s="34"/>
       <c r="H46" s="34"/>
       <c r="I46" s="34"/>
@@ -13819,10 +16045,10 @@
     <row r="47" spans="1:11" ht="13">
       <c r="A47" s="34"/>
       <c r="B47" s="34"/>
-      <c r="C47" s="81"/>
-      <c r="D47" s="81"/>
-      <c r="E47" s="81"/>
-      <c r="F47" s="81"/>
+      <c r="C47" s="86"/>
+      <c r="D47" s="86"/>
+      <c r="E47" s="86"/>
+      <c r="F47" s="86"/>
       <c r="G47" s="34"/>
       <c r="H47" s="34"/>
       <c r="I47" s="34"/>
@@ -14059,8 +16285,8 @@
   </sheetPr>
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -14611,12 +16837,12 @@
     <row r="32" spans="1:11" ht="13">
       <c r="A32" s="34"/>
       <c r="B32" s="34"/>
-      <c r="C32" s="82" t="s">
+      <c r="C32" s="87" t="s">
         <v>186</v>
       </c>
-      <c r="D32" s="81"/>
-      <c r="E32" s="81"/>
-      <c r="F32" s="81"/>
+      <c r="D32" s="86"/>
+      <c r="E32" s="86"/>
+      <c r="F32" s="86"/>
       <c r="G32" s="34"/>
       <c r="H32" s="34"/>
       <c r="I32" s="34"/>
@@ -14626,10 +16852,10 @@
     <row r="33" spans="1:11" ht="13">
       <c r="A33" s="34"/>
       <c r="B33" s="34"/>
-      <c r="C33" s="81"/>
-      <c r="D33" s="81"/>
-      <c r="E33" s="81"/>
-      <c r="F33" s="81"/>
+      <c r="C33" s="86"/>
+      <c r="D33" s="86"/>
+      <c r="E33" s="86"/>
+      <c r="F33" s="86"/>
       <c r="G33" s="34"/>
       <c r="H33" s="34"/>
       <c r="I33" s="34"/>
@@ -14639,10 +16865,10 @@
     <row r="34" spans="1:11" ht="13">
       <c r="A34" s="34"/>
       <c r="B34" s="34"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="81"/>
+      <c r="C34" s="86"/>
+      <c r="D34" s="86"/>
+      <c r="E34" s="86"/>
+      <c r="F34" s="86"/>
       <c r="G34" s="34"/>
       <c r="H34" s="34"/>
       <c r="I34" s="34"/>
@@ -14652,10 +16878,10 @@
     <row r="35" spans="1:11" ht="15.75" customHeight="1">
       <c r="A35" s="34"/>
       <c r="B35" s="34"/>
-      <c r="C35" s="81"/>
-      <c r="D35" s="81"/>
-      <c r="E35" s="81"/>
-      <c r="F35" s="81"/>
+      <c r="C35" s="86"/>
+      <c r="D35" s="86"/>
+      <c r="E35" s="86"/>
+      <c r="F35" s="86"/>
       <c r="G35" s="34"/>
       <c r="H35" s="34"/>
       <c r="I35" s="34"/>
@@ -14665,10 +16891,10 @@
     <row r="36" spans="1:11" ht="15.75" customHeight="1">
       <c r="A36" s="34"/>
       <c r="B36" s="34"/>
-      <c r="C36" s="81"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="81"/>
-      <c r="F36" s="81"/>
+      <c r="C36" s="86"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="86"/>
+      <c r="F36" s="86"/>
       <c r="G36" s="34"/>
       <c r="H36" s="34"/>
       <c r="I36" s="34"/>
@@ -14678,10 +16904,10 @@
     <row r="37" spans="1:11" ht="15.75" customHeight="1">
       <c r="A37" s="34"/>
       <c r="B37" s="34"/>
-      <c r="C37" s="81"/>
-      <c r="D37" s="81"/>
-      <c r="E37" s="81"/>
-      <c r="F37" s="81"/>
+      <c r="C37" s="86"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="86"/>
+      <c r="F37" s="86"/>
       <c r="G37" s="34"/>
       <c r="H37" s="42"/>
       <c r="I37" s="34"/>
@@ -14691,10 +16917,10 @@
     <row r="38" spans="1:11" ht="13">
       <c r="A38" s="34"/>
       <c r="B38" s="34"/>
-      <c r="C38" s="81"/>
-      <c r="D38" s="81"/>
-      <c r="E38" s="81"/>
-      <c r="F38" s="81"/>
+      <c r="C38" s="86"/>
+      <c r="D38" s="86"/>
+      <c r="E38" s="86"/>
+      <c r="F38" s="86"/>
       <c r="G38" s="34"/>
       <c r="H38" s="34"/>
       <c r="I38" s="34"/>
@@ -14704,10 +16930,10 @@
     <row r="39" spans="1:11" ht="15.75" customHeight="1">
       <c r="A39" s="34"/>
       <c r="B39" s="34"/>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="86"/>
+      <c r="F39" s="86"/>
       <c r="G39" s="34"/>
       <c r="H39" s="34"/>
       <c r="I39" s="34"/>
@@ -14717,10 +16943,10 @@
     <row r="40" spans="1:11" ht="15.75" customHeight="1">
       <c r="A40" s="34"/>
       <c r="B40" s="34"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="81"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="86"/>
+      <c r="E40" s="86"/>
+      <c r="F40" s="86"/>
       <c r="G40" s="34"/>
       <c r="H40" s="34"/>
       <c r="I40" s="34"/>
@@ -14730,10 +16956,10 @@
     <row r="41" spans="1:11" ht="13">
       <c r="A41" s="34"/>
       <c r="B41" s="34"/>
-      <c r="C41" s="81"/>
-      <c r="D41" s="81"/>
-      <c r="E41" s="81"/>
-      <c r="F41" s="81"/>
+      <c r="C41" s="86"/>
+      <c r="D41" s="86"/>
+      <c r="E41" s="86"/>
+      <c r="F41" s="86"/>
       <c r="G41" s="34"/>
       <c r="H41" s="34"/>
       <c r="I41" s="34"/>
@@ -14743,10 +16969,10 @@
     <row r="42" spans="1:11" ht="13">
       <c r="A42" s="34"/>
       <c r="B42" s="34"/>
-      <c r="C42" s="81"/>
-      <c r="D42" s="81"/>
-      <c r="E42" s="81"/>
-      <c r="F42" s="81"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="86"/>
+      <c r="E42" s="86"/>
+      <c r="F42" s="86"/>
       <c r="G42" s="34"/>
       <c r="H42" s="34"/>
       <c r="I42" s="34"/>
@@ -14756,10 +16982,10 @@
     <row r="43" spans="1:11" ht="13">
       <c r="A43" s="34"/>
       <c r="B43" s="34"/>
-      <c r="C43" s="81"/>
-      <c r="D43" s="81"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="81"/>
+      <c r="C43" s="86"/>
+      <c r="D43" s="86"/>
+      <c r="E43" s="86"/>
+      <c r="F43" s="86"/>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
       <c r="I43" s="34"/>
@@ -14769,10 +16995,10 @@
     <row r="44" spans="1:11" ht="13">
       <c r="A44" s="34"/>
       <c r="B44" s="34"/>
-      <c r="C44" s="81"/>
-      <c r="D44" s="81"/>
-      <c r="E44" s="81"/>
-      <c r="F44" s="81"/>
+      <c r="C44" s="86"/>
+      <c r="D44" s="86"/>
+      <c r="E44" s="86"/>
+      <c r="F44" s="86"/>
       <c r="G44" s="34"/>
       <c r="H44" s="34"/>
       <c r="I44" s="34"/>
@@ -15030,7 +17256,7 @@
   </sheetPr>
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -15572,12 +17798,12 @@
     <row r="32" spans="1:11" ht="13">
       <c r="A32" s="34"/>
       <c r="B32" s="34"/>
-      <c r="C32" s="80" t="s">
+      <c r="C32" s="85" t="s">
         <v>118</v>
       </c>
-      <c r="D32" s="81"/>
-      <c r="E32" s="81"/>
-      <c r="F32" s="81"/>
+      <c r="D32" s="86"/>
+      <c r="E32" s="86"/>
+      <c r="F32" s="86"/>
       <c r="G32" s="34"/>
       <c r="H32" s="34"/>
       <c r="I32" s="34"/>
@@ -15587,10 +17813,10 @@
     <row r="33" spans="1:11" ht="13">
       <c r="A33" s="34"/>
       <c r="B33" s="34"/>
-      <c r="C33" s="81"/>
-      <c r="D33" s="81"/>
-      <c r="E33" s="81"/>
-      <c r="F33" s="81"/>
+      <c r="C33" s="86"/>
+      <c r="D33" s="86"/>
+      <c r="E33" s="86"/>
+      <c r="F33" s="86"/>
       <c r="G33" s="34"/>
       <c r="H33" s="34"/>
       <c r="I33" s="34"/>
@@ -15600,10 +17826,10 @@
     <row r="34" spans="1:11" ht="13">
       <c r="A34" s="34"/>
       <c r="B34" s="34"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="81"/>
+      <c r="C34" s="86"/>
+      <c r="D34" s="86"/>
+      <c r="E34" s="86"/>
+      <c r="F34" s="86"/>
       <c r="G34" s="34"/>
       <c r="H34" s="34"/>
       <c r="I34" s="34"/>
@@ -15613,10 +17839,10 @@
     <row r="35" spans="1:11" ht="15.75" customHeight="1">
       <c r="A35" s="34"/>
       <c r="B35" s="34"/>
-      <c r="C35" s="81"/>
-      <c r="D35" s="81"/>
-      <c r="E35" s="81"/>
-      <c r="F35" s="81"/>
+      <c r="C35" s="86"/>
+      <c r="D35" s="86"/>
+      <c r="E35" s="86"/>
+      <c r="F35" s="86"/>
       <c r="G35" s="34"/>
       <c r="H35" s="34"/>
       <c r="I35" s="34"/>
@@ -15626,10 +17852,10 @@
     <row r="36" spans="1:11" ht="15.75" customHeight="1">
       <c r="A36" s="34"/>
       <c r="B36" s="34"/>
-      <c r="C36" s="81"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="81"/>
-      <c r="F36" s="81"/>
+      <c r="C36" s="86"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="86"/>
+      <c r="F36" s="86"/>
       <c r="G36" s="34"/>
       <c r="H36" s="34"/>
       <c r="I36" s="34"/>
@@ -15639,10 +17865,10 @@
     <row r="37" spans="1:11" ht="15.75" customHeight="1">
       <c r="A37" s="34"/>
       <c r="B37" s="34"/>
-      <c r="C37" s="81"/>
-      <c r="D37" s="81"/>
-      <c r="E37" s="81"/>
-      <c r="F37" s="81"/>
+      <c r="C37" s="86"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="86"/>
+      <c r="F37" s="86"/>
       <c r="G37" s="34"/>
       <c r="H37" s="42"/>
       <c r="I37" s="34"/>
@@ -15652,10 +17878,10 @@
     <row r="38" spans="1:11" ht="13">
       <c r="A38" s="34"/>
       <c r="B38" s="34"/>
-      <c r="C38" s="81"/>
-      <c r="D38" s="81"/>
-      <c r="E38" s="81"/>
-      <c r="F38" s="81"/>
+      <c r="C38" s="86"/>
+      <c r="D38" s="86"/>
+      <c r="E38" s="86"/>
+      <c r="F38" s="86"/>
       <c r="G38" s="34"/>
       <c r="H38" s="34"/>
       <c r="I38" s="34"/>
@@ -15665,10 +17891,10 @@
     <row r="39" spans="1:11" ht="15.75" customHeight="1">
       <c r="A39" s="34"/>
       <c r="B39" s="34"/>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="86"/>
+      <c r="F39" s="86"/>
       <c r="G39" s="34"/>
       <c r="H39" s="34"/>
       <c r="I39" s="34"/>
@@ -15678,10 +17904,10 @@
     <row r="40" spans="1:11" ht="15.75" customHeight="1">
       <c r="A40" s="34"/>
       <c r="B40" s="34"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="81"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="86"/>
+      <c r="E40" s="86"/>
+      <c r="F40" s="86"/>
       <c r="G40" s="34"/>
       <c r="H40" s="34"/>
       <c r="I40" s="34"/>
@@ -15691,10 +17917,10 @@
     <row r="41" spans="1:11" ht="13">
       <c r="A41" s="34"/>
       <c r="B41" s="34"/>
-      <c r="C41" s="81"/>
-      <c r="D41" s="81"/>
-      <c r="E41" s="81"/>
-      <c r="F41" s="81"/>
+      <c r="C41" s="86"/>
+      <c r="D41" s="86"/>
+      <c r="E41" s="86"/>
+      <c r="F41" s="86"/>
       <c r="G41" s="34"/>
       <c r="H41" s="34"/>
       <c r="I41" s="34"/>
@@ -15704,10 +17930,10 @@
     <row r="42" spans="1:11" ht="13">
       <c r="A42" s="34"/>
       <c r="B42" s="34"/>
-      <c r="C42" s="81"/>
-      <c r="D42" s="81"/>
-      <c r="E42" s="81"/>
-      <c r="F42" s="81"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="86"/>
+      <c r="E42" s="86"/>
+      <c r="F42" s="86"/>
       <c r="G42" s="34"/>
       <c r="H42" s="34"/>
       <c r="I42" s="34"/>
@@ -15717,10 +17943,10 @@
     <row r="43" spans="1:11" ht="13">
       <c r="A43" s="34"/>
       <c r="B43" s="34"/>
-      <c r="C43" s="81"/>
-      <c r="D43" s="81"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="81"/>
+      <c r="C43" s="86"/>
+      <c r="D43" s="86"/>
+      <c r="E43" s="86"/>
+      <c r="F43" s="86"/>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
       <c r="I43" s="34"/>
@@ -15730,10 +17956,10 @@
     <row r="44" spans="1:11" ht="13">
       <c r="A44" s="34"/>
       <c r="B44" s="34"/>
-      <c r="C44" s="81"/>
-      <c r="D44" s="81"/>
-      <c r="E44" s="81"/>
-      <c r="F44" s="81"/>
+      <c r="C44" s="86"/>
+      <c r="D44" s="86"/>
+      <c r="E44" s="86"/>
+      <c r="F44" s="86"/>
       <c r="G44" s="34"/>
       <c r="H44" s="34"/>
       <c r="I44" s="34"/>

</xml_diff>